<commit_message>
feat: Update `processa_medicoes.py` to support new `BASE.xlsx` value column and month formats, and add Pyright configuration.
</commit_message>
<xml_diff>
--- a/MEDIÇÕES_CONSOLIDADO.xlsx
+++ b/MEDIÇÕES_CONSOLIDADO.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
-  <workbookPr/>
+  <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDICOES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAB2219-8839-45CC-AC86-21FA59AFE947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CB7449-6F2E-4729-8644-A224BB3981FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1528,7 +1528,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{42C202FC-D074-456E-9E82-BDDE4205E08F}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{3AF75625-6D83-471F-899E-04980FAC3540}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1826,9 +1826,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:CK53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BY1" sqref="BY1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1844,11 +1847,11 @@
     <col min="10" max="10" width="8.42578125" customWidth="1"/>
     <col min="11" max="11" width="26.28515625" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
     <col min="16" max="16" width="8.5703125" customWidth="1"/>
-    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
     <col min="18" max="18" width="9.140625" customWidth="1"/>
     <col min="19" max="19" width="9.85546875" customWidth="1"/>
     <col min="20" max="20" width="9.42578125" customWidth="1"/>
@@ -3026,19 +3029,19 @@
         <v>107</v>
       </c>
       <c r="M5" s="7">
-        <v>2125804.48</v>
+        <v>2683515.34</v>
       </c>
       <c r="N5" s="4">
         <v>0</v>
       </c>
       <c r="O5" s="7">
-        <v>2125804.48</v>
+        <v>2683515.34</v>
       </c>
       <c r="P5" s="9">
-        <v>0.11194240337571321</v>
+        <v>0.14131081173335111</v>
       </c>
       <c r="Q5" s="7">
-        <v>16864358.460000001</v>
+        <v>16306647.6</v>
       </c>
       <c r="R5" s="7">
         <v>0</v>
@@ -3206,10 +3209,10 @@
         <v>0</v>
       </c>
       <c r="BU5" s="7">
-        <v>173.72</v>
+        <v>173719.79</v>
       </c>
       <c r="BV5" s="7">
-        <v>384.55</v>
+        <v>384549.34</v>
       </c>
       <c r="BW5" s="7">
         <v>747983.29</v>
@@ -3301,13 +3304,13 @@
         <v>0</v>
       </c>
       <c r="O6" s="7">
-        <v>7322834.1200000001</v>
+        <v>7070321.0300000003</v>
       </c>
       <c r="P6" s="9">
-        <v>0.86518531156782608</v>
+        <v>0.83535114997594706</v>
       </c>
       <c r="Q6" s="7">
-        <v>1141056.82</v>
+        <v>1393569.91</v>
       </c>
       <c r="R6" s="7">
         <v>0</v>
@@ -3367,7 +3370,7 @@
         <v>251528.78</v>
       </c>
       <c r="AK6" s="7">
-        <v>280570.09999999998</v>
+        <v>28057.01</v>
       </c>
       <c r="AL6" s="7">
         <v>241160.41</v>
@@ -3570,13 +3573,13 @@
         <v>0</v>
       </c>
       <c r="O7" s="7">
-        <v>1222003.4099999999</v>
+        <v>1145901.75</v>
       </c>
       <c r="P7" s="9">
-        <v>0.79927824590911789</v>
+        <v>0.74950227898642985</v>
       </c>
       <c r="Q7" s="7">
-        <v>306880.2</v>
+        <v>382981.86</v>
       </c>
       <c r="R7" s="7">
         <v>0</v>
@@ -3696,7 +3699,7 @@
         <v>0</v>
       </c>
       <c r="BE7" s="7">
-        <v>84557.4</v>
+        <v>8455.74</v>
       </c>
       <c r="BF7" s="7">
         <v>123108.53</v>
@@ -3833,19 +3836,19 @@
         <v>117</v>
       </c>
       <c r="M8" s="7">
-        <v>30458067.09</v>
+        <v>579644.25</v>
       </c>
       <c r="N8" s="4">
         <v>0</v>
       </c>
       <c r="O8" s="7">
-        <v>30766036.899999999</v>
+        <v>887614.06</v>
       </c>
       <c r="P8" s="9">
-        <v>9.3383280732226748</v>
+        <v>0.26941498255451801</v>
       </c>
       <c r="Q8" s="7">
-        <v>-27471438.91</v>
+        <v>2406983.9300000002</v>
       </c>
       <c r="R8" s="7">
         <v>0</v>
@@ -4010,10 +4013,10 @@
         <v>224011.87</v>
       </c>
       <c r="BT8" s="7">
-        <v>168073.5</v>
+        <v>16807.349999999999</v>
       </c>
       <c r="BU8" s="7">
-        <v>30027431</v>
+        <v>300274.31</v>
       </c>
       <c r="BV8" s="7">
         <v>0</v>
@@ -4102,19 +4105,19 @@
         <v>119</v>
       </c>
       <c r="M9" s="7">
-        <v>9079067.8699999992</v>
+        <v>7755221.3200000003</v>
       </c>
       <c r="N9" s="4">
         <v>0</v>
       </c>
       <c r="O9" s="7">
-        <v>30814130.48</v>
+        <v>29490283.93</v>
       </c>
       <c r="P9" s="9">
-        <v>0.50895720276765122</v>
+        <v>0.4870912202951318</v>
       </c>
       <c r="Q9" s="7">
-        <v>29729526.850000001</v>
+        <v>31053373.399999999</v>
       </c>
       <c r="R9" s="7">
         <v>0</v>
@@ -4261,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="BN9" s="7">
-        <v>-1572209.23</v>
+        <v>1572209.23</v>
       </c>
       <c r="BO9" s="7">
         <v>873599.05</v>
@@ -4276,7 +4279,7 @@
         <v>152909.82999999999</v>
       </c>
       <c r="BS9" s="7">
-        <v>4513399</v>
+        <v>45133.99</v>
       </c>
       <c r="BT9" s="7">
         <v>147679.79</v>
@@ -4371,19 +4374,19 @@
         <v>122</v>
       </c>
       <c r="M10" s="7">
-        <v>146046247.84</v>
+        <v>8583843.9700000007</v>
       </c>
       <c r="N10" s="4">
         <v>0</v>
       </c>
       <c r="O10" s="7">
-        <v>191796119.02000001</v>
+        <v>53244971.829999998</v>
       </c>
       <c r="P10" s="9">
-        <v>3.4133808959251439</v>
+        <v>0.94759670100333215</v>
       </c>
       <c r="Q10" s="7">
-        <v>-135606632.74000001</v>
+        <v>2944514.45</v>
       </c>
       <c r="R10" s="7">
         <v>0</v>
@@ -4467,16 +4470,16 @@
         <v>0</v>
       </c>
       <c r="AS10" s="7">
-        <v>820871.5</v>
+        <v>82087.149999999994</v>
       </c>
       <c r="AT10" s="7">
-        <v>179115.5</v>
+        <v>17911.55</v>
       </c>
       <c r="AU10" s="7">
         <v>2750605.37</v>
       </c>
       <c r="AV10" s="7">
-        <v>209727.8</v>
+        <v>20972.78</v>
       </c>
       <c r="AW10" s="7">
         <v>195003.86</v>
@@ -4545,19 +4548,19 @@
         <v>1575540.19</v>
       </c>
       <c r="BS10" s="7">
-        <v>93752891</v>
+        <v>937528.91</v>
       </c>
       <c r="BT10" s="7">
         <v>206718.42</v>
       </c>
       <c r="BU10" s="7">
-        <v>2014691</v>
+        <v>20146.91</v>
       </c>
       <c r="BV10" s="7">
-        <v>20566178</v>
+        <v>205661.78</v>
       </c>
       <c r="BW10" s="7">
-        <v>22517153</v>
+        <v>225171.53</v>
       </c>
       <c r="BX10" s="7">
         <v>974456.46</v>
@@ -4909,19 +4912,19 @@
         <v>128</v>
       </c>
       <c r="M12" s="7">
-        <v>1171602.8500000001</v>
+        <v>1739254.2</v>
       </c>
       <c r="N12" s="4">
         <v>0</v>
       </c>
       <c r="O12" s="7">
-        <v>1171602.8500000001</v>
+        <v>1739254.2</v>
       </c>
       <c r="P12" s="9">
-        <v>0.40958802900021618</v>
+        <v>0.60803684431831817</v>
       </c>
       <c r="Q12" s="7">
-        <v>1688839.27</v>
+        <v>1121187.92</v>
       </c>
       <c r="R12" s="7">
         <v>0</v>
@@ -5095,7 +5098,7 @@
         <v>243467.57</v>
       </c>
       <c r="BW12" s="7">
-        <v>568.22</v>
+        <v>568219.56999999995</v>
       </c>
       <c r="BX12" s="7">
         <v>584772.99</v>
@@ -5718,13 +5721,13 @@
         <v>0</v>
       </c>
       <c r="O15" s="7">
-        <v>6488132.9299999997</v>
+        <v>6205092.3799999999</v>
       </c>
       <c r="P15" s="9">
-        <v>0.84208591174083958</v>
+        <v>0.80535046532229981</v>
       </c>
       <c r="Q15" s="7">
-        <v>1216701.98</v>
+        <v>1499742.53</v>
       </c>
       <c r="R15" s="7">
         <v>0</v>
@@ -5847,7 +5850,7 @@
         <v>0</v>
       </c>
       <c r="BF15" s="7">
-        <v>314489.5</v>
+        <v>31448.95</v>
       </c>
       <c r="BG15" s="7">
         <v>88206.39</v>
@@ -5981,19 +5984,19 @@
         <v>138</v>
       </c>
       <c r="M16" s="7">
-        <v>10584628.26</v>
+        <v>10045837.32</v>
       </c>
       <c r="N16" s="4">
         <v>0</v>
       </c>
       <c r="O16" s="7">
-        <v>32294745.039999999</v>
+        <v>31523514.969999999</v>
       </c>
       <c r="P16" s="9">
-        <v>0.66029519484692689</v>
+        <v>0.64452670035310999</v>
       </c>
       <c r="Q16" s="7">
-        <v>16614811.310000001</v>
+        <v>17386041.379999999</v>
       </c>
       <c r="R16" s="7">
         <v>0</v>
@@ -6089,7 +6092,7 @@
         <v>604692.32999999996</v>
       </c>
       <c r="AW16" s="7">
-        <v>234787</v>
+        <v>2347.87</v>
       </c>
       <c r="AX16" s="7">
         <v>435109.34</v>
@@ -6167,7 +6170,7 @@
         <v>762624.41</v>
       </c>
       <c r="BW16" s="7">
-        <v>598656.6</v>
+        <v>59865.66</v>
       </c>
       <c r="BX16" s="7">
         <v>314589.38</v>
@@ -6788,13 +6791,13 @@
         <v>0</v>
       </c>
       <c r="O19" s="7">
-        <v>29783885.440000001</v>
+        <v>29693198.199999999</v>
       </c>
       <c r="P19" s="9">
-        <v>0.85924166998354012</v>
+        <v>0.85662541443485507</v>
       </c>
       <c r="Q19" s="7">
-        <v>4879104.59</v>
+        <v>4969791.83</v>
       </c>
       <c r="R19" s="7">
         <v>0</v>
@@ -6890,7 +6893,7 @@
         <v>0</v>
       </c>
       <c r="AW19" s="7">
-        <v>100763.6</v>
+        <v>10076.36</v>
       </c>
       <c r="AX19" s="7">
         <v>104212.78</v>
@@ -7320,19 +7323,19 @@
         <v>151</v>
       </c>
       <c r="M21" s="7">
-        <v>-720020.73</v>
+        <v>4712016.07</v>
       </c>
       <c r="N21" s="4">
         <v>0</v>
       </c>
       <c r="O21" s="7">
-        <v>20268911.379999999</v>
+        <v>28612913.760000002</v>
       </c>
       <c r="P21" s="9">
-        <v>0.30860777742323769</v>
+        <v>0.43565081298788411</v>
       </c>
       <c r="Q21" s="7">
-        <v>45409638.75</v>
+        <v>37065636.369999997</v>
       </c>
       <c r="R21" s="7">
         <v>0</v>
@@ -7401,7 +7404,7 @@
         <v>967768.24</v>
       </c>
       <c r="AN21" s="7">
-        <v>540452.9</v>
+        <v>54045.29</v>
       </c>
       <c r="AO21" s="7">
         <v>609973.01</v>
@@ -7425,31 +7428,31 @@
         <v>285800.96999999997</v>
       </c>
       <c r="AV21" s="7">
-        <v>-499897.23</v>
+        <v>499897.23</v>
       </c>
       <c r="AW21" s="7">
-        <v>-127585.61</v>
+        <v>127585.61</v>
       </c>
       <c r="AX21" s="7">
-        <v>-34252.28</v>
+        <v>34252.28</v>
       </c>
       <c r="AY21" s="7">
-        <v>-135219.39000000001</v>
+        <v>135219.39000000001</v>
       </c>
       <c r="AZ21" s="7">
-        <v>-273099.03000000003</v>
+        <v>273099.03000000003</v>
       </c>
       <c r="BA21" s="7">
-        <v>-60128.5</v>
+        <v>6012.85</v>
       </c>
       <c r="BB21" s="7">
-        <v>-508655.35999999999</v>
+        <v>508655.35999999999</v>
       </c>
       <c r="BC21" s="7">
-        <v>-56896.959999999999</v>
+        <v>56896.959999999999</v>
       </c>
       <c r="BD21" s="7">
-        <v>-30510.06</v>
+        <v>30510.06</v>
       </c>
       <c r="BE21" s="7">
         <v>59095.88</v>
@@ -7497,19 +7500,19 @@
         <v>0</v>
       </c>
       <c r="BT21" s="7">
-        <v>-229823.05</v>
+        <v>229823.05</v>
       </c>
       <c r="BU21" s="7">
         <v>14426.39</v>
       </c>
       <c r="BV21" s="7">
-        <v>-1114030.22</v>
+        <v>1114030.22</v>
       </c>
       <c r="BW21" s="7">
-        <v>-208164.15</v>
+        <v>208164.15</v>
       </c>
       <c r="BX21" s="7">
-        <v>-1164000.98</v>
+        <v>1164000.98</v>
       </c>
       <c r="BY21" s="7">
         <v>1981571.28</v>
@@ -7589,19 +7592,19 @@
         <v>153</v>
       </c>
       <c r="M22" s="7">
-        <v>63784869.149999999</v>
+        <v>8177086.2000000002</v>
       </c>
       <c r="N22" s="4">
         <v>0</v>
       </c>
       <c r="O22" s="7">
-        <v>77151512.159999996</v>
+        <v>21095002.079999998</v>
       </c>
       <c r="P22" s="9">
-        <v>1.329455555725344</v>
+        <v>0.36350379828114171</v>
       </c>
       <c r="Q22" s="7">
-        <v>-19119100.449999999</v>
+        <v>36937409.630000003</v>
       </c>
       <c r="R22" s="7">
         <v>0</v>
@@ -7709,7 +7712,7 @@
         <v>444020.59</v>
       </c>
       <c r="BA22" s="7">
-        <v>498585.7</v>
+        <v>49858.57</v>
       </c>
       <c r="BB22" s="7">
         <v>357750.39</v>
@@ -7769,13 +7772,13 @@
         <v>1607390.05</v>
       </c>
       <c r="BU22" s="7">
-        <v>999175.9</v>
+        <v>99917.59</v>
       </c>
       <c r="BV22" s="7">
         <v>1290254.3700000001</v>
       </c>
       <c r="BW22" s="7">
-        <v>55261136</v>
+        <v>552611.36</v>
       </c>
       <c r="BX22" s="7">
         <v>711780.84</v>
@@ -8396,19 +8399,19 @@
         <v>156</v>
       </c>
       <c r="M25" s="7">
-        <v>270421192.83999997</v>
+        <v>22867981.510000002</v>
       </c>
       <c r="N25" s="4">
         <v>0</v>
       </c>
       <c r="O25" s="7">
-        <v>282816936.56999999</v>
+        <v>35263725.240000002</v>
       </c>
       <c r="P25" s="9">
-        <v>6.166639269102042</v>
+        <v>0.76890258227510955</v>
       </c>
       <c r="Q25" s="7">
-        <v>-236954526.88</v>
+        <v>10598684.449999999</v>
       </c>
       <c r="R25" s="7">
         <v>0</v>
@@ -8561,7 +8564,7 @@
         <v>1505339.86</v>
       </c>
       <c r="BP25" s="7">
-        <v>591596.30000000005</v>
+        <v>59159.63</v>
       </c>
       <c r="BQ25" s="7">
         <v>762847.31</v>
@@ -8576,10 +8579,10 @@
         <v>3726349.31</v>
       </c>
       <c r="BU25" s="7">
-        <v>99996553</v>
+        <v>999965.53</v>
       </c>
       <c r="BV25" s="7">
-        <v>149519381</v>
+        <v>1495193.81</v>
       </c>
       <c r="BW25" s="7">
         <v>1968255.63</v>
@@ -8665,19 +8668,19 @@
         <v>161</v>
       </c>
       <c r="M26" s="7">
-        <v>29074764.920000002</v>
+        <v>2395066.71</v>
       </c>
       <c r="N26" s="4">
         <v>0</v>
       </c>
       <c r="O26" s="7">
-        <v>30264383.530000001</v>
+        <v>3584685.32</v>
       </c>
       <c r="P26" s="9">
-        <v>5.0301451077419364</v>
+        <v>0.59579893003002582</v>
       </c>
       <c r="Q26" s="7">
-        <v>-24247781.050000001</v>
+        <v>2431917.16</v>
       </c>
       <c r="R26" s="7">
         <v>0</v>
@@ -8845,10 +8848,10 @@
         <v>63622.18</v>
       </c>
       <c r="BU26" s="7">
-        <v>308.02999999999997</v>
+        <v>308032.59000000003</v>
       </c>
       <c r="BV26" s="7">
-        <v>27260023</v>
+        <v>272600.23</v>
       </c>
       <c r="BW26" s="7">
         <v>363497.25</v>
@@ -8934,19 +8937,19 @@
         <v>164</v>
       </c>
       <c r="M27" s="7">
-        <v>32251627.239999998</v>
+        <v>33128534.579999998</v>
       </c>
       <c r="N27" s="4">
         <v>0</v>
       </c>
       <c r="O27" s="7">
-        <v>44481827.090000004</v>
+        <v>45358734.43</v>
       </c>
       <c r="P27" s="9">
-        <v>0.86515650437322555</v>
+        <v>0.88221205578748352</v>
       </c>
       <c r="Q27" s="7">
-        <v>6932948</v>
+        <v>6056040.6600000001</v>
       </c>
       <c r="R27" s="7">
         <v>0</v>
@@ -9120,10 +9123,10 @@
         <v>2051589.9</v>
       </c>
       <c r="BW27" s="7">
-        <v>970.56</v>
+        <v>970563.95</v>
       </c>
       <c r="BX27" s="7">
-        <v>102984.5</v>
+        <v>10298.450000000001</v>
       </c>
       <c r="BY27" s="7">
         <v>3383264.9</v>
@@ -9203,19 +9206,19 @@
         <v>167</v>
       </c>
       <c r="M28" s="7">
-        <v>696098.64</v>
+        <v>2106573.67</v>
       </c>
       <c r="N28" s="4">
         <v>0</v>
       </c>
       <c r="O28" s="7">
-        <v>696098.64</v>
+        <v>2106573.67</v>
       </c>
       <c r="P28" s="9">
-        <v>0.26753357604824141</v>
+        <v>0.80962546794254309</v>
       </c>
       <c r="Q28" s="7">
-        <v>1905812.68</v>
+        <v>495337.65</v>
       </c>
       <c r="R28" s="7">
         <v>0</v>
@@ -9380,19 +9383,19 @@
         <v>9064.49</v>
       </c>
       <c r="BT28" s="7">
-        <v>460.1</v>
+        <v>460102.03</v>
       </c>
       <c r="BU28" s="7">
-        <v>608.69000000000005</v>
+        <v>608693.84</v>
       </c>
       <c r="BV28" s="7">
-        <v>396.21</v>
+        <v>396208.68</v>
       </c>
       <c r="BW28" s="7">
-        <v>126.57</v>
+        <v>126570.92</v>
       </c>
       <c r="BX28" s="7">
-        <v>199454.3</v>
+        <v>19945.43</v>
       </c>
       <c r="BY28" s="7">
         <v>129958.08</v>
@@ -9472,19 +9475,19 @@
         <v>170</v>
       </c>
       <c r="M29" s="7">
-        <v>5374833.7199999997</v>
+        <v>425261.4</v>
       </c>
       <c r="N29" s="4">
         <v>0</v>
       </c>
       <c r="O29" s="7">
-        <v>5374833.7199999997</v>
+        <v>425261.4</v>
       </c>
       <c r="P29" s="9">
         <v>0</v>
       </c>
       <c r="Q29" s="7">
-        <v>-5374833.7199999997</v>
+        <v>-425261.4</v>
       </c>
       <c r="R29" s="7">
         <v>0</v>
@@ -9658,7 +9661,7 @@
         <v>0</v>
       </c>
       <c r="BW29" s="7">
-        <v>4999568</v>
+        <v>49995.68</v>
       </c>
       <c r="BX29" s="7">
         <v>375265.72</v>
@@ -9741,19 +9744,19 @@
         <v>172</v>
       </c>
       <c r="M30" s="7">
-        <v>19557304.370000001</v>
+        <v>18958744.699999999</v>
       </c>
       <c r="N30" s="4">
         <v>0</v>
       </c>
       <c r="O30" s="7">
-        <v>19844966.530000001</v>
+        <v>19246406.859999999</v>
       </c>
       <c r="P30" s="9">
-        <v>0.69729677815165103</v>
+        <v>0.67626506067349024</v>
       </c>
       <c r="Q30" s="7">
-        <v>8614890.3800000008</v>
+        <v>9213450.0500000007</v>
       </c>
       <c r="R30" s="7">
         <v>0</v>
@@ -9912,7 +9915,7 @@
         <v>133461.04</v>
       </c>
       <c r="BR30" s="7">
-        <v>665066.30000000005</v>
+        <v>66506.63</v>
       </c>
       <c r="BS30" s="7">
         <v>1225871.8</v>
@@ -10010,19 +10013,19 @@
         <v>172</v>
       </c>
       <c r="M31" s="7">
-        <v>4765616.75</v>
+        <v>3976099.14</v>
       </c>
       <c r="N31" s="4">
         <v>0</v>
       </c>
       <c r="O31" s="7">
-        <v>35393053.43</v>
+        <v>32751450.57</v>
       </c>
       <c r="P31" s="9">
-        <v>0.77402181806380344</v>
+        <v>0.71625177422331798</v>
       </c>
       <c r="Q31" s="7">
-        <v>10333116.82</v>
+        <v>12974719.68</v>
       </c>
       <c r="R31" s="7">
         <v>0</v>
@@ -10109,13 +10112,13 @@
         <v>654423.03</v>
       </c>
       <c r="AT31" s="7">
-        <v>847458.4</v>
+        <v>84745.84</v>
       </c>
       <c r="AU31" s="7">
-        <v>996428.80000000005</v>
+        <v>99642.880000000005</v>
       </c>
       <c r="AV31" s="7">
-        <v>213985.3</v>
+        <v>21398.53</v>
       </c>
       <c r="AW31" s="7">
         <v>122099.63</v>
@@ -10190,16 +10193,16 @@
         <v>289529.71000000002</v>
       </c>
       <c r="BU31" s="7">
-        <v>532646.80000000005</v>
+        <v>53264.68</v>
       </c>
       <c r="BV31" s="7">
-        <v>485.17</v>
+        <v>485170.46</v>
       </c>
       <c r="BW31" s="7">
         <v>1012783.71</v>
       </c>
       <c r="BX31" s="7">
-        <v>883134.2</v>
+        <v>88313.42</v>
       </c>
       <c r="BY31" s="7">
         <v>837187.79</v>
@@ -10279,19 +10282,19 @@
         <v>172</v>
       </c>
       <c r="M32" s="7">
-        <v>7552664.6299999999</v>
+        <v>8061194.3200000003</v>
       </c>
       <c r="N32" s="4">
         <v>0</v>
       </c>
       <c r="O32" s="7">
-        <v>41239247.009999998</v>
+        <v>39541097.210000001</v>
       </c>
       <c r="P32" s="9">
-        <v>0.94160078089520194</v>
+        <v>0.90282754196168558</v>
       </c>
       <c r="Q32" s="7">
-        <v>2557707.9700000002</v>
+        <v>4255857.7699999996</v>
       </c>
       <c r="R32" s="7">
         <v>0</v>
@@ -10363,7 +10366,7 @@
         <v>904885.44</v>
       </c>
       <c r="AO32" s="7">
-        <v>727233.4</v>
+        <v>72723.34</v>
       </c>
       <c r="AP32" s="7">
         <v>0</v>
@@ -10387,7 +10390,7 @@
         <v>536795.13</v>
       </c>
       <c r="AW32" s="7">
-        <v>606470.69999999995</v>
+        <v>60647.07</v>
       </c>
       <c r="AX32" s="7">
         <v>608799.93999999994</v>
@@ -10402,10 +10405,10 @@
         <v>289836.99</v>
       </c>
       <c r="BB32" s="7">
-        <v>650306.5</v>
+        <v>65030.65</v>
       </c>
       <c r="BC32" s="7">
-        <v>467855.5</v>
+        <v>46785.55</v>
       </c>
       <c r="BD32" s="7">
         <v>951169.12</v>
@@ -10465,13 +10468,13 @@
         <v>1495738.36</v>
       </c>
       <c r="BW32" s="7">
-        <v>810.54</v>
+        <v>810543.05</v>
       </c>
       <c r="BX32" s="7">
         <v>210535.57</v>
       </c>
       <c r="BY32" s="7">
-        <v>334669.8</v>
+        <v>33466.980000000003</v>
       </c>
       <c r="BZ32" s="7">
         <v>0</v>
@@ -10548,19 +10551,19 @@
         <v>177</v>
       </c>
       <c r="M33" s="7">
-        <v>4600873.3499999996</v>
+        <v>3832747.11</v>
       </c>
       <c r="N33" s="4">
         <v>0</v>
       </c>
       <c r="O33" s="7">
-        <v>5991696.6600000001</v>
+        <v>5223570.42</v>
       </c>
       <c r="P33" s="9">
-        <v>0.88560255406636024</v>
+        <v>0.77206967705496121</v>
       </c>
       <c r="Q33" s="7">
-        <v>773975.63</v>
+        <v>1542101.87</v>
       </c>
       <c r="R33" s="7">
         <v>0</v>
@@ -10719,7 +10722,7 @@
         <v>1778629.34</v>
       </c>
       <c r="BR33" s="7">
-        <v>853473.6</v>
+        <v>85347.36</v>
       </c>
       <c r="BS33" s="7">
         <v>791806.64</v>
@@ -10817,19 +10820,19 @@
         <v>179</v>
       </c>
       <c r="M34" s="7">
-        <v>29095650.030000001</v>
+        <v>2362289.83</v>
       </c>
       <c r="N34" s="4">
         <v>0</v>
       </c>
       <c r="O34" s="7">
-        <v>39495083.289999999</v>
+        <v>12761723.09</v>
       </c>
       <c r="P34" s="9">
-        <v>1.7303324757684351</v>
+        <v>0.55910817423144876</v>
       </c>
       <c r="Q34" s="7">
-        <v>-16669941.970000001</v>
+        <v>10063418.23</v>
       </c>
       <c r="R34" s="7">
         <v>0</v>
@@ -11000,16 +11003,16 @@
         <v>0</v>
       </c>
       <c r="BV34" s="7">
-        <v>712.59</v>
+        <v>712587.61</v>
       </c>
       <c r="BW34" s="7">
-        <v>27365472</v>
+        <v>273654.71999999997</v>
       </c>
       <c r="BX34" s="7">
         <v>367117.37</v>
       </c>
       <c r="BY34" s="7">
-        <v>392686.6</v>
+        <v>39268.660000000003</v>
       </c>
       <c r="BZ34" s="7">
         <v>0</v>
@@ -11086,19 +11089,19 @@
         <v>179</v>
       </c>
       <c r="M35" s="7">
-        <v>3253833.79</v>
+        <v>3085620.1</v>
       </c>
       <c r="N35" s="4">
         <v>0</v>
       </c>
       <c r="O35" s="7">
-        <v>14348711.09</v>
+        <v>14180497.4</v>
       </c>
       <c r="P35" s="9">
-        <v>0.5413731816476729</v>
+        <v>0.53502652235675852</v>
       </c>
       <c r="Q35" s="7">
-        <v>12155577.59</v>
+        <v>12323791.279999999</v>
       </c>
       <c r="R35" s="7">
         <v>0</v>
@@ -11245,7 +11248,7 @@
         <v>0</v>
       </c>
       <c r="BN35" s="7">
-        <v>186904.1</v>
+        <v>18690.41</v>
       </c>
       <c r="BO35" s="7">
         <v>1214701.27</v>
@@ -11361,13 +11364,13 @@
         <v>0</v>
       </c>
       <c r="O36" s="7">
-        <v>15889085.539999999</v>
+        <v>14156092.16</v>
       </c>
       <c r="P36" s="9">
-        <v>0.79026474653072609</v>
+        <v>0.70407202192505791</v>
       </c>
       <c r="Q36" s="7">
-        <v>4216942.99</v>
+        <v>5949936.3700000001</v>
       </c>
       <c r="R36" s="7">
         <v>0</v>
@@ -11487,7 +11490,7 @@
         <v>0</v>
       </c>
       <c r="BE36" s="7">
-        <v>531243.19999999995</v>
+        <v>53124.32</v>
       </c>
       <c r="BF36" s="7">
         <v>111606.91</v>
@@ -11502,13 +11505,13 @@
         <v>751552.98</v>
       </c>
       <c r="BJ36" s="7">
-        <v>805000</v>
+        <v>80.5</v>
       </c>
       <c r="BK36" s="7">
         <v>630821.07999999996</v>
       </c>
       <c r="BL36" s="7">
-        <v>450000</v>
+        <v>45</v>
       </c>
       <c r="BM36" s="7">
         <v>0</v>
@@ -11630,13 +11633,13 @@
         <v>0</v>
       </c>
       <c r="O37" s="7">
-        <v>7571952.2800000003</v>
+        <v>6142640.3200000003</v>
       </c>
       <c r="P37" s="9">
-        <v>0.97130349876731292</v>
+        <v>0.78795637028039578</v>
       </c>
       <c r="Q37" s="7">
-        <v>223708.18</v>
+        <v>1653020.14</v>
       </c>
       <c r="R37" s="7">
         <v>0</v>
@@ -11714,7 +11717,7 @@
         <v>1055071.1200000001</v>
       </c>
       <c r="AQ37" s="7">
-        <v>523066.3</v>
+        <v>52306.63</v>
       </c>
       <c r="AR37" s="7">
         <v>1069722.6100000001</v>
@@ -11744,7 +11747,7 @@
         <v>170056.31</v>
       </c>
       <c r="BA37" s="7">
-        <v>279264</v>
+        <v>2792.64</v>
       </c>
       <c r="BB37" s="7">
         <v>0</v>
@@ -11762,13 +11765,13 @@
         <v>698367.68</v>
       </c>
       <c r="BG37" s="7">
-        <v>675950.2</v>
+        <v>67595.02</v>
       </c>
       <c r="BH37" s="7">
         <v>354120.32</v>
       </c>
       <c r="BI37" s="7">
-        <v>81917.5</v>
+        <v>8191.75</v>
       </c>
       <c r="BJ37" s="7">
         <v>224576.79</v>
@@ -12162,19 +12165,19 @@
         <v>190</v>
       </c>
       <c r="M39" s="7">
-        <v>19184635.260000002</v>
+        <v>4381697.88</v>
       </c>
       <c r="N39" s="4">
         <v>0</v>
       </c>
       <c r="O39" s="7">
-        <v>19184635.260000002</v>
+        <v>4381697.88</v>
       </c>
       <c r="P39" s="9">
-        <v>2.7147422476220582</v>
+        <v>0.62003682582141539</v>
       </c>
       <c r="Q39" s="7">
-        <v>-12117800.359999999</v>
+        <v>2685137.02</v>
       </c>
       <c r="R39" s="7">
         <v>0</v>
@@ -12345,10 +12348,10 @@
         <v>0</v>
       </c>
       <c r="BV39" s="7">
-        <v>7875757</v>
+        <v>78757.570000000007</v>
       </c>
       <c r="BW39" s="7">
-        <v>7076705</v>
+        <v>70767.05</v>
       </c>
       <c r="BX39" s="7">
         <v>24903.47</v>
@@ -12431,19 +12434,19 @@
         <v>192</v>
       </c>
       <c r="M40" s="7">
-        <v>2336764.75</v>
+        <v>2420969.38</v>
       </c>
       <c r="N40" s="4">
         <v>0</v>
       </c>
       <c r="O40" s="7">
-        <v>2336764.75</v>
+        <v>2420969.38</v>
       </c>
       <c r="P40" s="9">
-        <v>0.2257876679292608</v>
+        <v>0.23392386008833299</v>
       </c>
       <c r="Q40" s="7">
-        <v>8012625.7699999996</v>
+        <v>7928421.1399999997</v>
       </c>
       <c r="R40" s="7">
         <v>0</v>
@@ -12617,7 +12620,7 @@
         <v>0</v>
       </c>
       <c r="BW40" s="7">
-        <v>84.29</v>
+        <v>84288.92</v>
       </c>
       <c r="BX40" s="7">
         <v>272777.33</v>
@@ -12703,16 +12706,16 @@
         <v>13791452.859999999</v>
       </c>
       <c r="N41" s="4">
-        <v>0</v>
+        <v>7440875.0800000001</v>
       </c>
       <c r="O41" s="7">
-        <v>13791452.859999999</v>
+        <v>21232327.940000001</v>
       </c>
       <c r="P41" s="9">
-        <v>0.50270062348722733</v>
+        <v>0.7739216891702646</v>
       </c>
       <c r="Q41" s="7">
-        <v>13643271.140000001</v>
+        <v>6202396.0599999996</v>
       </c>
       <c r="R41" s="7">
         <v>0</v>
@@ -12895,7 +12898,7 @@
         <v>13791452.859999999</v>
       </c>
       <c r="BZ41" s="7">
-        <v>0</v>
+        <v>7440875.0800000001</v>
       </c>
       <c r="CA41" s="7">
         <v>0</v>
@@ -12969,19 +12972,19 @@
         <v>196</v>
       </c>
       <c r="M42" s="7">
-        <v>548089.31000000006</v>
+        <v>368496.83</v>
       </c>
       <c r="N42" s="4">
         <v>0</v>
       </c>
       <c r="O42" s="7">
-        <v>548089.31000000006</v>
+        <v>368496.83</v>
       </c>
       <c r="P42" s="9">
         <v>0</v>
       </c>
       <c r="Q42" s="7">
-        <v>-548089.31000000006</v>
+        <v>-368496.83</v>
       </c>
       <c r="R42" s="7">
         <v>0</v>
@@ -13140,7 +13143,7 @@
         <v>0</v>
       </c>
       <c r="BR42" s="7">
-        <v>21939.599999999999</v>
+        <v>2193.96</v>
       </c>
       <c r="BS42" s="7">
         <v>0</v>
@@ -13161,7 +13164,7 @@
         <v>233489.27</v>
       </c>
       <c r="BY42" s="7">
-        <v>177607.6</v>
+        <v>17760.759999999998</v>
       </c>
       <c r="BZ42" s="7">
         <v>0</v>
@@ -13238,19 +13241,19 @@
         <v>198</v>
       </c>
       <c r="M43" s="7">
-        <v>132088.35999999999</v>
+        <v>164482.69</v>
       </c>
       <c r="N43" s="4">
         <v>0</v>
       </c>
       <c r="O43" s="7">
-        <v>132088.35999999999</v>
+        <v>164482.69</v>
       </c>
       <c r="P43" s="9">
         <v>0</v>
       </c>
       <c r="Q43" s="7">
-        <v>-132088.35999999999</v>
+        <v>-164482.69</v>
       </c>
       <c r="R43" s="7">
         <v>0</v>
@@ -13421,7 +13424,7 @@
         <v>0</v>
       </c>
       <c r="BV43" s="7">
-        <v>32.43</v>
+        <v>32426.76</v>
       </c>
       <c r="BW43" s="7">
         <v>52055.93</v>
@@ -13782,13 +13785,13 @@
         <v>0</v>
       </c>
       <c r="O45" s="7">
-        <v>2301268.7200000002</v>
+        <v>2270712.37</v>
       </c>
       <c r="P45" s="9">
-        <v>0.15136457559011721</v>
+        <v>0.14935474991911379</v>
       </c>
       <c r="Q45" s="7">
-        <v>12902214.07</v>
+        <v>12932770.42</v>
       </c>
       <c r="R45" s="7">
         <v>0</v>
@@ -13923,7 +13926,7 @@
         <v>64140.14</v>
       </c>
       <c r="BJ45" s="7">
-        <v>30865</v>
+        <v>308.64999999999998</v>
       </c>
       <c r="BK45" s="7">
         <v>53092.18</v>
@@ -14045,19 +14048,19 @@
         <v>206</v>
       </c>
       <c r="M46" s="7">
-        <v>245984367.97</v>
+        <v>11147804.810000001</v>
       </c>
       <c r="N46" s="4">
         <v>0</v>
       </c>
       <c r="O46" s="7">
-        <v>245984367.97</v>
+        <v>11147804.810000001</v>
       </c>
       <c r="P46" s="9">
-        <v>10.16991235714991</v>
+        <v>0.46089188035778339</v>
       </c>
       <c r="Q46" s="7">
-        <v>-221796906.03999999</v>
+        <v>13039657.119999999</v>
       </c>
       <c r="R46" s="7">
         <v>0</v>
@@ -14216,7 +14219,7 @@
         <v>93817.279999999999</v>
       </c>
       <c r="BR46" s="7">
-        <v>302.27</v>
+        <v>302267.46000000002</v>
       </c>
       <c r="BS46" s="7">
         <v>1205629.77</v>
@@ -14225,13 +14228,13 @@
         <v>1125037.28</v>
       </c>
       <c r="BU46" s="7">
-        <v>227136775</v>
+        <v>2271367.75</v>
       </c>
       <c r="BV46" s="7">
         <v>1358528.8</v>
       </c>
       <c r="BW46" s="7">
-        <v>11414579</v>
+        <v>1141457.8999999999</v>
       </c>
       <c r="BX46" s="7">
         <v>1199347.44</v>
@@ -14314,19 +14317,19 @@
         <v>130</v>
       </c>
       <c r="M47" s="7">
-        <v>10432387.09</v>
+        <v>10511270.470000001</v>
       </c>
       <c r="N47" s="4">
         <v>0</v>
       </c>
       <c r="O47" s="7">
-        <v>10432387.09</v>
+        <v>10511270.470000001</v>
       </c>
       <c r="P47" s="9">
-        <v>0.83912383021845705</v>
+        <v>0.84546877537771292</v>
       </c>
       <c r="Q47" s="7">
-        <v>2000089.16</v>
+        <v>1921205.78</v>
       </c>
       <c r="R47" s="7">
         <v>0</v>
@@ -14497,7 +14500,7 @@
         <v>0</v>
       </c>
       <c r="BV47" s="7">
-        <v>78.959999999999994</v>
+        <v>78962.34</v>
       </c>
       <c r="BW47" s="7">
         <v>2207726.0099999998</v>
@@ -14583,19 +14586,19 @@
         <v>210</v>
       </c>
       <c r="M48" s="7">
-        <v>26589011.350000001</v>
+        <v>10301084.52</v>
       </c>
       <c r="N48" s="4">
         <v>0</v>
       </c>
       <c r="O48" s="7">
-        <v>26589011.350000001</v>
+        <v>10301084.52</v>
       </c>
       <c r="P48" s="9">
-        <v>2.1974166898110599</v>
+        <v>0.851320673395491</v>
       </c>
       <c r="Q48" s="7">
-        <v>-14488888.75</v>
+        <v>1799038.08</v>
       </c>
       <c r="R48" s="7">
         <v>0</v>
@@ -14757,7 +14760,7 @@
         <v>0</v>
       </c>
       <c r="BS48" s="7">
-        <v>106.38</v>
+        <v>106382.54</v>
       </c>
       <c r="BT48" s="7">
         <v>413616.54</v>
@@ -14766,7 +14769,7 @@
         <v>192392.13</v>
       </c>
       <c r="BV48" s="7">
-        <v>16559801</v>
+        <v>165598.01</v>
       </c>
       <c r="BW48" s="7">
         <v>2318891.39</v>
@@ -14858,13 +14861,13 @@
         <v>0</v>
       </c>
       <c r="O49" s="7">
-        <v>56075179.539999999</v>
+        <v>55215321.43</v>
       </c>
       <c r="P49" s="9">
-        <v>0.94803871360320457</v>
+        <v>0.93350146587305349</v>
       </c>
       <c r="Q49" s="7">
-        <v>3073438.27</v>
+        <v>3933296.38</v>
       </c>
       <c r="R49" s="7">
         <v>0</v>
@@ -14984,7 +14987,7 @@
         <v>187923.63</v>
       </c>
       <c r="BE49" s="7">
-        <v>515128.1</v>
+        <v>51512.81</v>
       </c>
       <c r="BF49" s="7">
         <v>142691.85999999999</v>
@@ -15008,7 +15011,7 @@
         <v>1021876.31</v>
       </c>
       <c r="BM49" s="7">
-        <v>440269.8</v>
+        <v>44026.98</v>
       </c>
       <c r="BN49" s="7">
         <v>1729073.23</v>
@@ -15390,19 +15393,19 @@
         <v>153</v>
       </c>
       <c r="M51" s="7">
-        <v>37185511.390000001</v>
+        <v>12334165.09</v>
       </c>
       <c r="N51" s="4">
         <v>0</v>
       </c>
       <c r="O51" s="7">
-        <v>63590015.32</v>
+        <v>38672688.490000002</v>
       </c>
       <c r="P51" s="9">
-        <v>1.5267250368280489</v>
+        <v>0.92848793103789629</v>
       </c>
       <c r="Q51" s="7">
-        <v>-21938759.34</v>
+        <v>2978567.49</v>
       </c>
       <c r="R51" s="7">
         <v>0</v>
@@ -15522,7 +15525,7 @@
         <v>0</v>
       </c>
       <c r="BE51" s="7">
-        <v>66647</v>
+        <v>666.47</v>
       </c>
       <c r="BF51" s="7">
         <v>7823810.8099999996</v>
@@ -15573,10 +15576,10 @@
         <v>152137.68</v>
       </c>
       <c r="BV51" s="7">
-        <v>12040881</v>
+        <v>120408.81</v>
       </c>
       <c r="BW51" s="7">
-        <v>13061489</v>
+        <v>130614.89</v>
       </c>
       <c r="BX51" s="7">
         <v>1108417.1399999999</v>
@@ -15659,19 +15662,19 @@
         <v>217</v>
       </c>
       <c r="M52" s="7">
-        <v>26360257.239999998</v>
+        <v>54247300.539999999</v>
       </c>
       <c r="N52" s="4">
         <v>0</v>
       </c>
       <c r="O52" s="7">
-        <v>26360257.239999998</v>
+        <v>54247300.539999999</v>
       </c>
       <c r="P52" s="9">
-        <v>0.25119419090171308</v>
+        <v>0.5169375489655641</v>
       </c>
       <c r="Q52" s="7">
-        <v>78579499.310000002</v>
+        <v>50692456.009999998</v>
       </c>
       <c r="R52" s="7">
         <v>0</v>
@@ -15839,7 +15842,7 @@
         <v>0</v>
       </c>
       <c r="BU52" s="7">
-        <v>0</v>
+        <v>27887043.300000001</v>
       </c>
       <c r="BV52" s="7">
         <v>3</v>
@@ -15928,19 +15931,19 @@
         <v>219</v>
       </c>
       <c r="M53" s="7">
-        <v>145443451.81999999</v>
+        <v>53528793.799999997</v>
       </c>
       <c r="N53" s="4">
         <v>0</v>
       </c>
       <c r="O53" s="7">
-        <v>152181593.38999999</v>
+        <v>60266935.369999997</v>
       </c>
       <c r="P53" s="9">
-        <v>2.0397045353547831</v>
+        <v>0.80776353215789232</v>
       </c>
       <c r="Q53" s="7">
-        <v>-77571966.969999999</v>
+        <v>14342691.050000001</v>
       </c>
       <c r="R53" s="7">
         <v>0</v>
@@ -16093,7 +16096,7 @@
         <v>380731.29</v>
       </c>
       <c r="BP53" s="7">
-        <v>941725.7</v>
+        <v>94172.57</v>
       </c>
       <c r="BQ53" s="7">
         <v>7173927.79</v>
@@ -16102,10 +16105,10 @@
         <v>4408318.83</v>
       </c>
       <c r="BS53" s="7">
-        <v>91182265</v>
+        <v>911822.65</v>
       </c>
       <c r="BT53" s="7">
-        <v>797460</v>
+        <v>797.46</v>
       </c>
       <c r="BU53" s="7">
         <v>4046951.13</v>
@@ -16166,6 +16169,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:CK116"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16565,13 +16569,13 @@
         <v>0</v>
       </c>
       <c r="O2" s="7">
-        <v>67821381.790000007</v>
+        <v>985523.15</v>
       </c>
       <c r="P2" s="9">
-        <v>55.935980941114188</v>
+        <v>0.81281452368690832</v>
       </c>
       <c r="Q2" s="7">
-        <v>-66608899.579999998</v>
+        <v>226959.06</v>
       </c>
       <c r="R2" s="7">
         <v>0</v>
@@ -16586,19 +16590,19 @@
         <v>0</v>
       </c>
       <c r="V2" s="7">
-        <v>11005384</v>
+        <v>110053.84</v>
       </c>
       <c r="W2" s="7">
-        <v>17011677</v>
+        <v>170116.77</v>
       </c>
       <c r="X2" s="7">
-        <v>17003346</v>
+        <v>170033.46</v>
       </c>
       <c r="Y2" s="7">
-        <v>10330286</v>
+        <v>0</v>
       </c>
       <c r="Z2" s="7">
-        <v>12055929</v>
+        <v>120559.29</v>
       </c>
       <c r="AA2" s="7">
         <v>176585.58</v>
@@ -16832,13 +16836,13 @@
         <v>0</v>
       </c>
       <c r="O3" s="7">
-        <v>75957961.340000004</v>
+        <v>75473224.310000002</v>
       </c>
       <c r="P3" s="9">
-        <v>0.89907733560078806</v>
+        <v>0.89333973983451076</v>
       </c>
       <c r="Q3" s="7">
-        <v>8526385.3699999992</v>
+        <v>9011122.4000000004</v>
       </c>
       <c r="R3" s="7">
         <v>0</v>
@@ -16907,7 +16911,7 @@
         <v>411572.18</v>
       </c>
       <c r="AN3" s="7">
-        <v>538596.69999999995</v>
+        <v>53859.67</v>
       </c>
       <c r="AO3" s="7">
         <v>0</v>
@@ -17099,13 +17103,13 @@
         <v>0</v>
       </c>
       <c r="O4" s="7">
-        <v>32682339.390000001</v>
+        <v>31828130.850000001</v>
       </c>
       <c r="P4" s="9">
-        <v>0.47058804017278622</v>
+        <v>0.45828842116630669</v>
       </c>
       <c r="Q4" s="7">
-        <v>36767660.609999999</v>
+        <v>37621869.149999999</v>
       </c>
       <c r="R4" s="7">
         <v>0</v>
@@ -17165,13 +17169,13 @@
         <v>2268052.17</v>
       </c>
       <c r="AK4" s="7">
-        <v>524475.5</v>
+        <v>52447.55</v>
       </c>
       <c r="AL4" s="7">
         <v>955557.19</v>
       </c>
       <c r="AM4" s="7">
-        <v>386041</v>
+        <v>3860.41</v>
       </c>
       <c r="AN4" s="7">
         <v>391310.72</v>
@@ -18438,13 +18442,13 @@
         <v>0</v>
       </c>
       <c r="O9" s="7">
-        <v>8394719</v>
+        <v>8075594.0300000003</v>
       </c>
       <c r="P9" s="9">
-        <v>0.99981054057729291</v>
+        <v>0.96180277536592462</v>
       </c>
       <c r="Q9" s="7">
-        <v>1590.76</v>
+        <v>320715.73</v>
       </c>
       <c r="R9" s="7">
         <v>0</v>
@@ -18570,7 +18574,7 @@
         <v>36613.279999999999</v>
       </c>
       <c r="BG9" s="7">
-        <v>354583.3</v>
+        <v>35458.33</v>
       </c>
       <c r="BH9" s="7">
         <v>403701.68</v>
@@ -18707,13 +18711,13 @@
         <v>0</v>
       </c>
       <c r="O10" s="7">
-        <v>4374443.7300000004</v>
+        <v>3921891.87</v>
       </c>
       <c r="P10" s="9">
-        <v>0.99999998856997541</v>
+        <v>0.89654641075304886</v>
       </c>
       <c r="Q10" s="7">
-        <v>0.05</v>
+        <v>452551.91</v>
       </c>
       <c r="R10" s="7">
         <v>0</v>
@@ -18779,7 +18783,7 @@
         <v>107650.53</v>
       </c>
       <c r="AM10" s="7">
-        <v>183183.2</v>
+        <v>18318.32</v>
       </c>
       <c r="AN10" s="7">
         <v>798369.63</v>
@@ -18800,7 +18804,7 @@
         <v>139028.48000000001</v>
       </c>
       <c r="AT10" s="7">
-        <v>319652.2</v>
+        <v>31965.22</v>
       </c>
       <c r="AU10" s="7">
         <v>296228.71999999997</v>
@@ -18976,13 +18980,13 @@
         <v>0</v>
       </c>
       <c r="O11" s="7">
-        <v>1740561.74</v>
+        <v>1712039.39</v>
       </c>
       <c r="P11" s="9">
-        <v>0.9993443488656788</v>
+        <v>0.9829682280801737</v>
       </c>
       <c r="Q11" s="7">
-        <v>1141.95</v>
+        <v>29664.3</v>
       </c>
       <c r="R11" s="7">
         <v>0</v>
@@ -19096,7 +19100,7 @@
         <v>0</v>
       </c>
       <c r="BC11" s="7">
-        <v>31691.5</v>
+        <v>3169.15</v>
       </c>
       <c r="BD11" s="7">
         <v>0</v>
@@ -19245,13 +19249,13 @@
         <v>0</v>
       </c>
       <c r="O12" s="7">
-        <v>7104640.0499999998</v>
+        <v>6138303.75</v>
       </c>
       <c r="P12" s="9">
-        <v>0.80625685039546691</v>
+        <v>0.69659397427821601</v>
       </c>
       <c r="Q12" s="7">
-        <v>1707241.73</v>
+        <v>2673578.0299999998</v>
       </c>
       <c r="R12" s="7">
         <v>0</v>
@@ -19347,7 +19351,7 @@
         <v>686049.52</v>
       </c>
       <c r="AW12" s="7">
-        <v>416125.5</v>
+        <v>41612.550000000003</v>
       </c>
       <c r="AX12" s="7">
         <v>409515.77</v>
@@ -19362,7 +19366,7 @@
         <v>597793.73</v>
       </c>
       <c r="BB12" s="7">
-        <v>112805.2</v>
+        <v>11280.52</v>
       </c>
       <c r="BC12" s="7">
         <v>185864.99</v>
@@ -19380,10 +19384,10 @@
         <v>617746.35</v>
       </c>
       <c r="BH12" s="7">
-        <v>525255.5</v>
+        <v>52525.55</v>
       </c>
       <c r="BI12" s="7">
-        <v>19520.8</v>
+        <v>1952.08</v>
       </c>
       <c r="BJ12" s="7">
         <v>0</v>
@@ -19781,13 +19785,13 @@
         <v>0</v>
       </c>
       <c r="O14" s="7">
-        <v>5132338.3099999996</v>
+        <v>4942414.46</v>
       </c>
       <c r="P14" s="9">
-        <v>0.9734912273243751</v>
+        <v>0.93746686753608399</v>
       </c>
       <c r="Q14" s="7">
-        <v>139756.76999999999</v>
+        <v>329680.62</v>
       </c>
       <c r="R14" s="7">
         <v>0</v>
@@ -19907,7 +19911,7 @@
         <v>0</v>
       </c>
       <c r="BE14" s="7">
-        <v>211026.5</v>
+        <v>21102.65</v>
       </c>
       <c r="BF14" s="7">
         <v>827</v>
@@ -20050,13 +20054,13 @@
         <v>0</v>
       </c>
       <c r="O15" s="7">
-        <v>4625557.49</v>
+        <v>3542960.18</v>
       </c>
       <c r="P15" s="9">
-        <v>0.99578167540148987</v>
+        <v>0.7627220787004344</v>
       </c>
       <c r="Q15" s="7">
-        <v>19594.759999999998</v>
+        <v>1102192.07</v>
       </c>
       <c r="R15" s="7">
         <v>0</v>
@@ -20152,7 +20156,7 @@
         <v>140614.75</v>
       </c>
       <c r="AW15" s="7">
-        <v>319668.5</v>
+        <v>31966.85</v>
       </c>
       <c r="AX15" s="7">
         <v>164215.32999999999</v>
@@ -20176,7 +20180,7 @@
         <v>120984.77</v>
       </c>
       <c r="BE15" s="7">
-        <v>883217.4</v>
+        <v>88321.74</v>
       </c>
       <c r="BF15" s="7">
         <v>492856.12</v>
@@ -20317,13 +20321,13 @@
         <v>0</v>
       </c>
       <c r="O16" s="7">
-        <v>3607318.65</v>
+        <v>3129510</v>
       </c>
       <c r="P16" s="9">
-        <v>0.999986480445621</v>
+        <v>0.86753292238803892</v>
       </c>
       <c r="Q16" s="7">
-        <v>48.77</v>
+        <v>477857.42</v>
       </c>
       <c r="R16" s="7">
         <v>0</v>
@@ -20398,7 +20402,7 @@
         <v>468162.08</v>
       </c>
       <c r="AP16" s="7">
-        <v>482635</v>
+        <v>4826.3500000000004</v>
       </c>
       <c r="AQ16" s="7">
         <v>150829.29</v>
@@ -20586,13 +20590,13 @@
         <v>0</v>
       </c>
       <c r="O17" s="7">
-        <v>10939879.359999999</v>
+        <v>10246752.91</v>
       </c>
       <c r="P17" s="9">
-        <v>0.99033797691154157</v>
+        <v>0.92759236302966441</v>
       </c>
       <c r="Q17" s="7">
-        <v>106732.62</v>
+        <v>799859.07</v>
       </c>
       <c r="R17" s="7">
         <v>0</v>
@@ -20664,7 +20668,7 @@
         <v>484641.18</v>
       </c>
       <c r="AO17" s="7">
-        <v>490457.4</v>
+        <v>49045.74</v>
       </c>
       <c r="AP17" s="7">
         <v>655903.26</v>
@@ -20691,7 +20695,7 @@
         <v>100847.74</v>
       </c>
       <c r="AX17" s="7">
-        <v>279683.09999999998</v>
+        <v>27968.31</v>
       </c>
       <c r="AY17" s="7">
         <v>0</v>
@@ -21122,13 +21126,13 @@
         <v>0</v>
       </c>
       <c r="O19" s="7">
-        <v>6171355.1699999999</v>
+        <v>5982279.4800000004</v>
       </c>
       <c r="P19" s="9">
-        <v>0.20344279465159371</v>
+        <v>0.19720978979047851</v>
       </c>
       <c r="Q19" s="7">
-        <v>24163241.739999998</v>
+        <v>24352317.43</v>
       </c>
       <c r="R19" s="7">
         <v>0</v>
@@ -21212,7 +21216,7 @@
         <v>1076635.31</v>
       </c>
       <c r="AS19" s="7">
-        <v>210084.1</v>
+        <v>21008.41</v>
       </c>
       <c r="AT19" s="7">
         <v>1160220.94</v>
@@ -21385,19 +21389,19 @@
         <v>117</v>
       </c>
       <c r="M20" s="7">
-        <v>2214379.38</v>
+        <v>2044683.93</v>
       </c>
       <c r="N20" s="4">
         <v>0</v>
       </c>
       <c r="O20" s="7">
-        <v>10061305.060000001</v>
+        <v>9339511</v>
       </c>
       <c r="P20" s="9">
-        <v>1.0000297833057219</v>
+        <v>0.92828804074760951</v>
       </c>
       <c r="Q20" s="7">
-        <v>-299.64999999999998</v>
+        <v>721494.41</v>
       </c>
       <c r="R20" s="7">
         <v>0</v>
@@ -21508,7 +21512,7 @@
         <v>163311.32</v>
       </c>
       <c r="BB20" s="7">
-        <v>67907.3</v>
+        <v>6790.73</v>
       </c>
       <c r="BC20" s="7">
         <v>631326.01</v>
@@ -21529,7 +21533,7 @@
         <v>1225723.92</v>
       </c>
       <c r="BI20" s="7">
-        <v>545535.6</v>
+        <v>54553.56</v>
       </c>
       <c r="BJ20" s="7">
         <v>811014.79</v>
@@ -21553,7 +21557,7 @@
         <v>53970.74</v>
       </c>
       <c r="BQ20" s="7">
-        <v>188550.5</v>
+        <v>18855.05</v>
       </c>
       <c r="BR20" s="7">
         <v>1482105.79</v>
@@ -21654,19 +21658,19 @@
         <v>263</v>
       </c>
       <c r="M21" s="7">
-        <v>91471127.849999994</v>
+        <v>5971037.2300000004</v>
       </c>
       <c r="N21" s="4">
         <v>0</v>
       </c>
       <c r="O21" s="7">
-        <v>117814518.31999999</v>
+        <v>28986729.09</v>
       </c>
       <c r="P21" s="9">
-        <v>3.6289959806947141</v>
+        <v>0.89286723623805864</v>
       </c>
       <c r="Q21" s="7">
-        <v>-85349748.739999995</v>
+        <v>3478040.49</v>
       </c>
       <c r="R21" s="7">
         <v>0</v>
@@ -21723,7 +21727,7 @@
         <v>531985.32999999996</v>
       </c>
       <c r="AJ21" s="7">
-        <v>945681.4</v>
+        <v>94568.14</v>
       </c>
       <c r="AK21" s="7">
         <v>806675.88</v>
@@ -21738,7 +21742,7 @@
         <v>1228434.6000000001</v>
       </c>
       <c r="AO21" s="7">
-        <v>471895.2</v>
+        <v>47189.52</v>
       </c>
       <c r="AP21" s="7">
         <v>1027729.48</v>
@@ -21762,7 +21766,7 @@
         <v>0</v>
       </c>
       <c r="AW21" s="7">
-        <v>916009.5</v>
+        <v>91600.95</v>
       </c>
       <c r="AX21" s="7">
         <v>641381.87</v>
@@ -21789,10 +21793,10 @@
         <v>1315203.06</v>
       </c>
       <c r="BF21" s="7">
-        <v>904326.6</v>
+        <v>90432.66</v>
       </c>
       <c r="BG21" s="7">
-        <v>459530.2</v>
+        <v>45953.02</v>
       </c>
       <c r="BH21" s="7">
         <v>1726518.92</v>
@@ -21828,19 +21832,19 @@
         <v>490205.36</v>
       </c>
       <c r="BS21" s="7">
-        <v>300.11</v>
+        <v>300112.44</v>
       </c>
       <c r="BT21" s="7">
         <v>245695.84</v>
       </c>
       <c r="BU21" s="7">
-        <v>19842363</v>
+        <v>198423.63</v>
       </c>
       <c r="BV21" s="7">
-        <v>418.84</v>
+        <v>418843.69</v>
       </c>
       <c r="BW21" s="7">
-        <v>67246857</v>
+        <v>672468.57</v>
       </c>
       <c r="BX21" s="7">
         <v>0</v>
@@ -21929,13 +21933,13 @@
         <v>0</v>
       </c>
       <c r="O22" s="7">
-        <v>17677149.640000001</v>
+        <v>16552659.939999999</v>
       </c>
       <c r="P22" s="9">
-        <v>0.99898742458747924</v>
+        <v>0.93543922296812876</v>
       </c>
       <c r="Q22" s="7">
-        <v>17917.59</v>
+        <v>1142407.29</v>
       </c>
       <c r="R22" s="7">
         <v>0</v>
@@ -22043,7 +22047,7 @@
         <v>2109380.2200000002</v>
       </c>
       <c r="BA22" s="7">
-        <v>799899.5</v>
+        <v>79989.95</v>
       </c>
       <c r="BB22" s="7">
         <v>1139276.74</v>
@@ -22076,7 +22080,7 @@
         <v>497948.46</v>
       </c>
       <c r="BL22" s="7">
-        <v>449533.5</v>
+        <v>44953.35</v>
       </c>
       <c r="BM22" s="7">
         <v>0</v>
@@ -24067,13 +24071,13 @@
         <v>0</v>
       </c>
       <c r="O30" s="7">
-        <v>4324004.79</v>
+        <v>3710200.11</v>
       </c>
       <c r="P30" s="9">
-        <v>0.97282670563476759</v>
+        <v>0.83473120996636385</v>
       </c>
       <c r="Q30" s="7">
-        <v>120779.43</v>
+        <v>734584.11</v>
       </c>
       <c r="R30" s="7">
         <v>0</v>
@@ -24187,7 +24191,7 @@
         <v>0</v>
       </c>
       <c r="BC30" s="7">
-        <v>682005.2</v>
+        <v>68200.52</v>
       </c>
       <c r="BD30" s="7">
         <v>550395.17000000004</v>
@@ -24603,13 +24607,13 @@
         <v>0</v>
       </c>
       <c r="O32" s="7">
-        <v>2226331.4500000002</v>
+        <v>2123652.9700000002</v>
       </c>
       <c r="P32" s="9">
-        <v>0.80792838834121261</v>
+        <v>0.77066670438857143</v>
       </c>
       <c r="Q32" s="7">
-        <v>529273.48</v>
+        <v>631951.96</v>
       </c>
       <c r="R32" s="7">
         <v>0</v>
@@ -24696,7 +24700,7 @@
         <v>0</v>
       </c>
       <c r="AT32" s="7">
-        <v>84942.1</v>
+        <v>8494.2099999999991</v>
       </c>
       <c r="AU32" s="7">
         <v>264382.34999999998</v>
@@ -24705,7 +24709,7 @@
         <v>28562.41</v>
       </c>
       <c r="AW32" s="7">
-        <v>29145.1</v>
+        <v>2914.51</v>
       </c>
       <c r="AX32" s="7">
         <v>30777.79</v>
@@ -24872,13 +24876,13 @@
         <v>0</v>
       </c>
       <c r="O33" s="7">
-        <v>56408430.850000001</v>
+        <v>55344940</v>
       </c>
       <c r="P33" s="9">
-        <v>0.9711077021977591</v>
+        <v>0.95279901783817922</v>
       </c>
       <c r="Q33" s="7">
-        <v>1678257.91</v>
+        <v>2741748.76</v>
       </c>
       <c r="R33" s="7">
         <v>0</v>
@@ -25007,7 +25011,7 @@
         <v>1957520.83</v>
       </c>
       <c r="BH33" s="7">
-        <v>779479</v>
+        <v>7794.79</v>
       </c>
       <c r="BI33" s="7">
         <v>5970935.7800000003</v>
@@ -25019,7 +25023,7 @@
         <v>4118696.93</v>
       </c>
       <c r="BL33" s="7">
-        <v>324229.59999999998</v>
+        <v>32422.959999999999</v>
       </c>
       <c r="BM33" s="7">
         <v>0</v>
@@ -25133,13 +25137,13 @@
         <v>0</v>
       </c>
       <c r="O34" s="7">
-        <v>123264139.69</v>
+        <v>8661926.9800000004</v>
       </c>
       <c r="P34" s="9">
-        <v>6.4886489830835057</v>
+        <v>0.45596556980537822</v>
       </c>
       <c r="Q34" s="7">
-        <v>-104267251.43000001</v>
+        <v>10334961.279999999</v>
       </c>
       <c r="R34" s="7">
         <v>0</v>
@@ -25259,19 +25263,19 @@
         <v>0</v>
       </c>
       <c r="BE34" s="7">
-        <v>11234312</v>
+        <v>112343.12</v>
       </c>
       <c r="BF34" s="7">
-        <v>33218693</v>
+        <v>332186.93</v>
       </c>
       <c r="BG34" s="7">
         <v>1076227.52</v>
       </c>
       <c r="BH34" s="7">
-        <v>70943301</v>
+        <v>709433.01</v>
       </c>
       <c r="BI34" s="7">
-        <v>360230</v>
+        <v>360.23</v>
       </c>
       <c r="BJ34" s="7">
         <v>5622526.8099999996</v>
@@ -25934,13 +25938,13 @@
         <v>0</v>
       </c>
       <c r="O37" s="7">
-        <v>2389346</v>
+        <v>1883519.36</v>
       </c>
       <c r="P37" s="9">
-        <v>1</v>
+        <v>0.78829912453031081</v>
       </c>
       <c r="Q37" s="7">
-        <v>0</v>
+        <v>505826.64</v>
       </c>
       <c r="R37" s="7">
         <v>0</v>
@@ -26006,7 +26010,7 @@
         <v>739920.75</v>
       </c>
       <c r="AM37" s="7">
-        <v>562029.6</v>
+        <v>56202.96</v>
       </c>
       <c r="AN37" s="7">
         <v>0</v>
@@ -26203,13 +26207,13 @@
         <v>0</v>
       </c>
       <c r="O38" s="7">
-        <v>9661616.3699999992</v>
+        <v>9228959.0999999996</v>
       </c>
       <c r="P38" s="9">
-        <v>0.99077076080670301</v>
+        <v>0.94640301154504913</v>
       </c>
       <c r="Q38" s="7">
-        <v>90000</v>
+        <v>522657.27</v>
       </c>
       <c r="R38" s="7">
         <v>0</v>
@@ -26281,7 +26285,7 @@
         <v>261649.94</v>
       </c>
       <c r="AO38" s="7">
-        <v>65929.600000000006</v>
+        <v>6592.96</v>
       </c>
       <c r="AP38" s="7">
         <v>0</v>
@@ -26317,7 +26321,7 @@
         <v>536257.61</v>
       </c>
       <c r="BA38" s="7">
-        <v>414800.7</v>
+        <v>41480.07</v>
       </c>
       <c r="BB38" s="7">
         <v>0</v>
@@ -26472,13 +26476,13 @@
         <v>0</v>
       </c>
       <c r="O39" s="7">
-        <v>13792679.65</v>
+        <v>13384606.060000001</v>
       </c>
       <c r="P39" s="9">
-        <v>0.9999999898496883</v>
+        <v>0.97041374582654627</v>
       </c>
       <c r="Q39" s="7">
-        <v>0.14000000000000001</v>
+        <v>408073.73</v>
       </c>
       <c r="R39" s="7">
         <v>0</v>
@@ -26577,7 +26581,7 @@
         <v>280408.63</v>
       </c>
       <c r="AX39" s="7">
-        <v>304269.59999999998</v>
+        <v>30426.959999999999</v>
       </c>
       <c r="AY39" s="7">
         <v>186166.26</v>
@@ -26595,7 +26599,7 @@
         <v>108879.08</v>
       </c>
       <c r="BD39" s="7">
-        <v>149145.5</v>
+        <v>14914.55</v>
       </c>
       <c r="BE39" s="7">
         <v>0</v>
@@ -26739,13 +26743,13 @@
         <v>0</v>
       </c>
       <c r="O40" s="7">
-        <v>1003381821.37</v>
+        <v>74305044.280000001</v>
       </c>
       <c r="P40" s="9">
-        <v>12.45626306165696</v>
+        <v>0.922443638749605</v>
       </c>
       <c r="Q40" s="7">
-        <v>-922829426.45000005</v>
+        <v>6247350.6399999997</v>
       </c>
       <c r="R40" s="7">
         <v>0</v>
@@ -26850,7 +26854,7 @@
         <v>10433757.939999999</v>
       </c>
       <c r="AZ40" s="7">
-        <v>938461391</v>
+        <v>9384613.9100000001</v>
       </c>
       <c r="BA40" s="7">
         <v>0</v>
@@ -27006,13 +27010,13 @@
         <v>0</v>
       </c>
       <c r="O41" s="7">
-        <v>6453162.3300000001</v>
+        <v>5654932.8899999997</v>
       </c>
       <c r="P41" s="9">
-        <v>0.99999993956451794</v>
+        <v>0.87630409077922644</v>
       </c>
       <c r="Q41" s="7">
-        <v>0.39</v>
+        <v>798229.83</v>
       </c>
       <c r="R41" s="7">
         <v>0</v>
@@ -27072,7 +27076,7 @@
         <v>991327.11</v>
       </c>
       <c r="AK41" s="7">
-        <v>886921.6</v>
+        <v>88692.160000000003</v>
       </c>
       <c r="AL41" s="7">
         <v>1009464.43</v>
@@ -28349,13 +28353,13 @@
         <v>0</v>
       </c>
       <c r="O46" s="7">
-        <v>6450491.3099999996</v>
+        <v>5852661.0899999999</v>
       </c>
       <c r="P46" s="9">
-        <v>0.89161885674039276</v>
+        <v>0.80898380280970883</v>
       </c>
       <c r="Q46" s="7">
-        <v>784092.46</v>
+        <v>1381922.68</v>
       </c>
       <c r="R46" s="7">
         <v>0</v>
@@ -28487,7 +28491,7 @@
         <v>1940010.25</v>
       </c>
       <c r="BI46" s="7">
-        <v>664255.80000000005</v>
+        <v>66425.58</v>
       </c>
       <c r="BJ46" s="7">
         <v>531746.06000000006</v>
@@ -28618,13 +28622,13 @@
         <v>0</v>
       </c>
       <c r="O47" s="7">
-        <v>11566431.390000001</v>
+        <v>9534048.5099999998</v>
       </c>
       <c r="P47" s="9">
-        <v>0.9208715549510299</v>
+        <v>0.75906161376384984</v>
       </c>
       <c r="Q47" s="7">
-        <v>993877.73</v>
+        <v>3026260.61</v>
       </c>
       <c r="R47" s="7">
         <v>0</v>
@@ -28690,7 +28694,7 @@
         <v>0</v>
       </c>
       <c r="AM47" s="7">
-        <v>530861.6</v>
+        <v>53086.16</v>
       </c>
       <c r="AN47" s="7">
         <v>1760492.78</v>
@@ -28723,7 +28727,7 @@
         <v>836628.45</v>
       </c>
       <c r="AX47" s="7">
-        <v>798646.8</v>
+        <v>79864.679999999993</v>
       </c>
       <c r="AY47" s="7">
         <v>623254.15</v>
@@ -28732,13 +28736,13 @@
         <v>522476.34</v>
       </c>
       <c r="BA47" s="7">
-        <v>499145</v>
+        <v>4991.45</v>
       </c>
       <c r="BB47" s="7">
         <v>308370.59000000003</v>
       </c>
       <c r="BC47" s="7">
-        <v>379635.3</v>
+        <v>37963.53</v>
       </c>
       <c r="BD47" s="7">
         <v>801291.31</v>
@@ -28887,13 +28891,13 @@
         <v>0</v>
       </c>
       <c r="O48" s="7">
-        <v>20500685.690000001</v>
+        <v>19435944.559999999</v>
       </c>
       <c r="P48" s="9">
-        <v>0.9122436576489874</v>
+        <v>0.86486459152563766</v>
       </c>
       <c r="Q48" s="7">
-        <v>1972132.31</v>
+        <v>3036873.44</v>
       </c>
       <c r="R48" s="7">
         <v>0</v>
@@ -28992,7 +28996,7 @@
         <v>325739.93</v>
       </c>
       <c r="AX48" s="7">
-        <v>246359.8</v>
+        <v>24635.98</v>
       </c>
       <c r="AY48" s="7">
         <v>362421.28</v>
@@ -29007,7 +29011,7 @@
         <v>1052655.1299999999</v>
       </c>
       <c r="BC48" s="7">
-        <v>737884.2</v>
+        <v>73788.42</v>
       </c>
       <c r="BD48" s="7">
         <v>885986.93</v>
@@ -29019,7 +29023,7 @@
         <v>522414.47</v>
       </c>
       <c r="BG48" s="7">
-        <v>198801.7</v>
+        <v>19880.169999999998</v>
       </c>
       <c r="BH48" s="7">
         <v>0</v>
@@ -29156,13 +29160,13 @@
         <v>0</v>
       </c>
       <c r="O49" s="7">
-        <v>43785880.079999998</v>
+        <v>43141110.719999999</v>
       </c>
       <c r="P49" s="9">
-        <v>0.9679090660784373</v>
+        <v>0.9536561126620996</v>
       </c>
       <c r="Q49" s="7">
-        <v>1451716.73</v>
+        <v>2096486.09</v>
       </c>
       <c r="R49" s="7">
         <v>0</v>
@@ -29240,7 +29244,7 @@
         <v>1156896.75</v>
       </c>
       <c r="AQ49" s="7">
-        <v>716410.4</v>
+        <v>71641.039999999994</v>
       </c>
       <c r="AR49" s="7">
         <v>788781.45</v>
@@ -29961,13 +29965,13 @@
         <v>0</v>
       </c>
       <c r="O52" s="7">
-        <v>151308</v>
+        <v>15130.8</v>
       </c>
       <c r="P52" s="9">
-        <v>1.3163589415629879E-2</v>
+        <v>1.316358941562987E-3</v>
       </c>
       <c r="Q52" s="7">
-        <v>11343125.26</v>
+        <v>11479302.460000001</v>
       </c>
       <c r="R52" s="7">
         <v>0</v>
@@ -30087,10 +30091,10 @@
         <v>0</v>
       </c>
       <c r="BE52" s="7">
-        <v>81485.399999999994</v>
+        <v>8148.54</v>
       </c>
       <c r="BF52" s="7">
-        <v>69822.600000000006</v>
+        <v>6982.26</v>
       </c>
       <c r="BG52" s="7">
         <v>0</v>
@@ -30230,13 +30234,13 @@
         <v>0</v>
       </c>
       <c r="O53" s="7">
-        <v>13332401.6</v>
+        <v>12433273.43</v>
       </c>
       <c r="P53" s="9">
-        <v>0.66050584967494952</v>
+        <v>0.61596178074347274</v>
       </c>
       <c r="Q53" s="7">
-        <v>6852736.21</v>
+        <v>7751864.3799999999</v>
       </c>
       <c r="R53" s="7">
         <v>0</v>
@@ -30302,10 +30306,10 @@
         <v>459809.72</v>
       </c>
       <c r="AM53" s="7">
-        <v>190282.7</v>
+        <v>19028.27</v>
       </c>
       <c r="AN53" s="7">
-        <v>396347.3</v>
+        <v>39634.730000000003</v>
       </c>
       <c r="AO53" s="7">
         <v>730556.69</v>
@@ -30326,7 +30330,7 @@
         <v>831397.29</v>
       </c>
       <c r="AU53" s="7">
-        <v>412401.3</v>
+        <v>41240.129999999997</v>
       </c>
       <c r="AV53" s="7">
         <v>428339.32</v>
@@ -30499,13 +30503,13 @@
         <v>0</v>
       </c>
       <c r="O54" s="7">
-        <v>12534756.699999999</v>
+        <v>11638364.17</v>
       </c>
       <c r="P54" s="9">
-        <v>0.4112759495442489</v>
+        <v>0.38186455387351192</v>
       </c>
       <c r="Q54" s="7">
-        <v>17942971.73</v>
+        <v>18839364.260000002</v>
       </c>
       <c r="R54" s="7">
         <v>0</v>
@@ -30562,7 +30566,7 @@
         <v>954009.41</v>
       </c>
       <c r="AJ54" s="7">
-        <v>905447</v>
+        <v>9054.4699999999993</v>
       </c>
       <c r="AK54" s="7">
         <v>0</v>
@@ -30768,13 +30772,13 @@
         <v>0</v>
       </c>
       <c r="O55" s="7">
-        <v>6523029.6600000001</v>
+        <v>5792351.6100000003</v>
       </c>
       <c r="P55" s="9">
-        <v>1.0069403748270731</v>
+        <v>0.8941478124911052</v>
       </c>
       <c r="Q55" s="7">
-        <v>-44960.23</v>
+        <v>685717.82</v>
       </c>
       <c r="R55" s="7">
         <v>0</v>
@@ -30861,7 +30865,7 @@
         <v>191164.06</v>
       </c>
       <c r="AT55" s="7">
-        <v>392087.9</v>
+        <v>39208.79</v>
       </c>
       <c r="AU55" s="7">
         <v>176656.04</v>
@@ -30891,7 +30895,7 @@
         <v>61458.43</v>
       </c>
       <c r="BD55" s="7">
-        <v>419776.6</v>
+        <v>41977.66</v>
       </c>
       <c r="BE55" s="7">
         <v>0</v>
@@ -31037,13 +31041,13 @@
         <v>0</v>
       </c>
       <c r="O56" s="7">
-        <v>6007931.0199999996</v>
+        <v>5144130.55</v>
       </c>
       <c r="P56" s="9">
-        <v>0.99217901617233051</v>
+        <v>0.8495267956923096</v>
       </c>
       <c r="Q56" s="7">
-        <v>47358.32</v>
+        <v>911158.79</v>
       </c>
       <c r="R56" s="7">
         <v>0</v>
@@ -31106,7 +31110,7 @@
         <v>1162941.93</v>
       </c>
       <c r="AL56" s="7">
-        <v>959778.3</v>
+        <v>95977.83</v>
       </c>
       <c r="AM56" s="7">
         <v>357381.39</v>
@@ -31306,13 +31310,13 @@
         <v>0</v>
       </c>
       <c r="O57" s="7">
-        <v>5551029.21</v>
+        <v>4601510.3099999996</v>
       </c>
       <c r="P57" s="9">
-        <v>0.97001638343982832</v>
+        <v>0.80409239807752408</v>
       </c>
       <c r="Q57" s="7">
-        <v>171584.66</v>
+        <v>1121103.56</v>
       </c>
       <c r="R57" s="7">
         <v>0</v>
@@ -31402,10 +31406,10 @@
         <v>340146.38</v>
       </c>
       <c r="AU57" s="7">
-        <v>779036.1</v>
+        <v>77903.61</v>
       </c>
       <c r="AV57" s="7">
-        <v>275984.90000000002</v>
+        <v>27598.49</v>
       </c>
       <c r="AW57" s="7">
         <v>49212.09</v>
@@ -31575,13 +31579,13 @@
         <v>0</v>
       </c>
       <c r="O58" s="7">
-        <v>5580983.9400000004</v>
+        <v>4936315.0199999996</v>
       </c>
       <c r="P58" s="9">
-        <v>0.99986610605924375</v>
+        <v>0.88436987642167597</v>
       </c>
       <c r="Q58" s="7">
-        <v>747.36</v>
+        <v>645416.28</v>
       </c>
       <c r="R58" s="7">
         <v>0</v>
@@ -31674,7 +31678,7 @@
         <v>46981.97</v>
       </c>
       <c r="AV58" s="7">
-        <v>137894.6</v>
+        <v>13789.46</v>
       </c>
       <c r="AW58" s="7">
         <v>92670.48</v>
@@ -31692,7 +31696,7 @@
         <v>0</v>
       </c>
       <c r="BB58" s="7">
-        <v>525822</v>
+        <v>5258.22</v>
       </c>
       <c r="BC58" s="7">
         <v>0</v>
@@ -31844,13 +31848,13 @@
         <v>0</v>
       </c>
       <c r="O59" s="7">
-        <v>12032786.93</v>
+        <v>11186461.67</v>
       </c>
       <c r="P59" s="9">
-        <v>0.91096529299621554</v>
+        <v>0.8468926103391482</v>
       </c>
       <c r="Q59" s="7">
-        <v>1176044.43</v>
+        <v>2022369.69</v>
       </c>
       <c r="R59" s="7">
         <v>0</v>
@@ -31934,7 +31938,7 @@
         <v>1476783.27</v>
       </c>
       <c r="AS59" s="7">
-        <v>940361.4</v>
+        <v>94036.14</v>
       </c>
       <c r="AT59" s="7">
         <v>603293.64</v>
@@ -32113,13 +32117,13 @@
         <v>0</v>
       </c>
       <c r="O60" s="7">
-        <v>8552770.9100000001</v>
+        <v>8494636.8499999996</v>
       </c>
       <c r="P60" s="9">
-        <v>0.6604266220686813</v>
+        <v>0.65593763466600818</v>
       </c>
       <c r="Q60" s="7">
-        <v>4397601.8099999996</v>
+        <v>4455735.87</v>
       </c>
       <c r="R60" s="7">
         <v>0</v>
@@ -32209,7 +32213,7 @@
         <v>0</v>
       </c>
       <c r="AU60" s="7">
-        <v>64593.4</v>
+        <v>6459.34</v>
       </c>
       <c r="AV60" s="7">
         <v>59504.88</v>
@@ -32645,19 +32649,19 @@
         <v>144</v>
       </c>
       <c r="M62" s="7">
-        <v>13491482.439999999</v>
+        <v>12776757.41</v>
       </c>
       <c r="N62" s="4">
         <v>0</v>
       </c>
       <c r="O62" s="7">
-        <v>80971534.769999996</v>
+        <v>80256809.739999995</v>
       </c>
       <c r="P62" s="9">
-        <v>0.9880484105351427</v>
+        <v>0.97932703787168629</v>
       </c>
       <c r="Q62" s="7">
-        <v>979444.46</v>
+        <v>1694169.49</v>
       </c>
       <c r="R62" s="7">
         <v>0</v>
@@ -32807,7 +32811,7 @@
         <v>344977.36</v>
       </c>
       <c r="BO62" s="7">
-        <v>902936.1</v>
+        <v>90293.61</v>
       </c>
       <c r="BP62" s="7">
         <v>2195846.5499999998</v>
@@ -32828,7 +32832,7 @@
         <v>1106666.3700000001</v>
       </c>
       <c r="BV62" s="7">
-        <v>989.07</v>
+        <v>98906.53</v>
       </c>
       <c r="BW62" s="7">
         <v>1004285.95</v>
@@ -32918,13 +32922,13 @@
         <v>0</v>
       </c>
       <c r="O63" s="7">
-        <v>2042159.29</v>
+        <v>1674266.74</v>
       </c>
       <c r="P63" s="9">
-        <v>0.22756440390169769</v>
+        <v>0.1865689491149041</v>
       </c>
       <c r="Q63" s="7">
-        <v>6931824.5800000001</v>
+        <v>7299717.1299999999</v>
       </c>
       <c r="R63" s="7">
         <v>0</v>
@@ -32987,7 +32991,7 @@
         <v>679501.38</v>
       </c>
       <c r="AL63" s="7">
-        <v>408769.5</v>
+        <v>40876.949999999997</v>
       </c>
       <c r="AM63" s="7">
         <v>382552.94</v>
@@ -33185,13 +33189,13 @@
         <v>0</v>
       </c>
       <c r="O64" s="7">
-        <v>4852080.3</v>
+        <v>3334970.55</v>
       </c>
       <c r="P64" s="9">
-        <v>0.40675264373232362</v>
+        <v>0.27957247285910358</v>
       </c>
       <c r="Q64" s="7">
-        <v>7076742.7199999997</v>
+        <v>8593852.4700000007</v>
       </c>
       <c r="R64" s="7">
         <v>0</v>
@@ -33269,7 +33273,7 @@
         <v>719239.45</v>
       </c>
       <c r="AQ64" s="7">
-        <v>721480</v>
+        <v>721.48</v>
       </c>
       <c r="AR64" s="7">
         <v>611174.84</v>
@@ -33281,7 +33285,7 @@
         <v>711229.41</v>
       </c>
       <c r="AU64" s="7">
-        <v>884834.7</v>
+        <v>88483.47</v>
       </c>
       <c r="AV64" s="7">
         <v>0</v>
@@ -33454,13 +33458,13 @@
         <v>0</v>
       </c>
       <c r="O65" s="7">
-        <v>11551184.42</v>
+        <v>10511349.710000001</v>
       </c>
       <c r="P65" s="9">
-        <v>0.99999999826857588</v>
+        <v>0.9099802504755089</v>
       </c>
       <c r="Q65" s="7">
-        <v>0.02</v>
+        <v>1039834.73</v>
       </c>
       <c r="R65" s="7">
         <v>0</v>
@@ -33520,7 +33524,7 @@
         <v>120478.62</v>
       </c>
       <c r="AK65" s="7">
-        <v>357653.7</v>
+        <v>35765.370000000003</v>
       </c>
       <c r="AL65" s="7">
         <v>730489.17</v>
@@ -33553,7 +33557,7 @@
         <v>743481.86</v>
       </c>
       <c r="AV65" s="7">
-        <v>205750.7</v>
+        <v>20575.07</v>
       </c>
       <c r="AW65" s="7">
         <v>207806.97</v>
@@ -33574,7 +33578,7 @@
         <v>1898281</v>
       </c>
       <c r="BC65" s="7">
-        <v>591967.5</v>
+        <v>59196.75</v>
       </c>
       <c r="BD65" s="7">
         <v>307578.92</v>
@@ -33717,19 +33721,19 @@
         <v>343</v>
       </c>
       <c r="M66" s="7">
-        <v>213257377.22</v>
+        <v>14120676.050000001</v>
       </c>
       <c r="N66" s="4">
         <v>0</v>
       </c>
       <c r="O66" s="7">
-        <v>240653017.94999999</v>
+        <v>41516316.780000001</v>
       </c>
       <c r="P66" s="9">
-        <v>5.4509092422761496</v>
+        <v>0.94036499840772703</v>
       </c>
       <c r="Q66" s="7">
-        <v>-196503866.44999999</v>
+        <v>2632834.7200000002</v>
       </c>
       <c r="R66" s="7">
         <v>0</v>
@@ -33900,10 +33904,10 @@
         <v>1823824.53</v>
       </c>
       <c r="BV66" s="7">
-        <v>126716316</v>
+        <v>1267163.1599999999</v>
       </c>
       <c r="BW66" s="7">
-        <v>74431867</v>
+        <v>744318.67</v>
       </c>
       <c r="BX66" s="7">
         <v>0</v>
@@ -33990,13 +33994,13 @@
         <v>0</v>
       </c>
       <c r="O67" s="7">
-        <v>1496414.32</v>
+        <v>1284066.97</v>
       </c>
       <c r="P67" s="9">
-        <v>0.99841264983394018</v>
+        <v>0.85673378618960183</v>
       </c>
       <c r="Q67" s="7">
-        <v>2379.11</v>
+        <v>214726.46</v>
       </c>
       <c r="R67" s="7">
         <v>0</v>
@@ -34065,7 +34069,7 @@
         <v>160691.98000000001</v>
       </c>
       <c r="AN67" s="7">
-        <v>235941.5</v>
+        <v>23594.15</v>
       </c>
       <c r="AO67" s="7">
         <v>293959.24</v>
@@ -34795,13 +34799,13 @@
         <v>0</v>
       </c>
       <c r="O70" s="7">
-        <v>18264452.890000001</v>
+        <v>17793137.829999998</v>
       </c>
       <c r="P70" s="9">
-        <v>1</v>
+        <v>0.97419495328775751</v>
       </c>
       <c r="Q70" s="7">
-        <v>0</v>
+        <v>471315.06</v>
       </c>
       <c r="R70" s="7">
         <v>0</v>
@@ -34939,7 +34943,7 @@
         <v>371421.96</v>
       </c>
       <c r="BK70" s="7">
-        <v>523683.4</v>
+        <v>52368.34</v>
       </c>
       <c r="BL70" s="7">
         <v>595765.34</v>
@@ -35333,13 +35337,13 @@
         <v>0</v>
       </c>
       <c r="O72" s="7">
-        <v>35196032.93</v>
+        <v>34668428.539999999</v>
       </c>
       <c r="P72" s="9">
-        <v>0.95433387945279813</v>
+        <v>0.9400279846570283</v>
       </c>
       <c r="Q72" s="7">
-        <v>1684176.07</v>
+        <v>2211780.46</v>
       </c>
       <c r="R72" s="7">
         <v>0</v>
@@ -35411,7 +35415,7 @@
         <v>2115661.2400000002</v>
       </c>
       <c r="AO72" s="7">
-        <v>586227.1</v>
+        <v>58622.71</v>
       </c>
       <c r="AP72" s="7">
         <v>646953.63</v>
@@ -35602,13 +35606,13 @@
         <v>0</v>
       </c>
       <c r="O73" s="7">
-        <v>19910338.670000002</v>
+        <v>18836010.379999999</v>
       </c>
       <c r="P73" s="9">
-        <v>0.98424001387554128</v>
+        <v>0.93113208293664029</v>
       </c>
       <c r="Q73" s="7">
-        <v>318811.12</v>
+        <v>1393139.41</v>
       </c>
       <c r="R73" s="7">
         <v>0</v>
@@ -35698,7 +35702,7 @@
         <v>483077.81</v>
       </c>
       <c r="AU73" s="7">
-        <v>504017.4</v>
+        <v>50401.74</v>
       </c>
       <c r="AV73" s="7">
         <v>498014.43</v>
@@ -35743,7 +35747,7 @@
         <v>848344.54</v>
       </c>
       <c r="BJ73" s="7">
-        <v>689680.7</v>
+        <v>68968.070000000007</v>
       </c>
       <c r="BK73" s="7">
         <v>398856.19</v>
@@ -36941,13 +36945,13 @@
         <v>0</v>
       </c>
       <c r="O78" s="7">
-        <v>12576165.07</v>
+        <v>12334318.960000001</v>
       </c>
       <c r="P78" s="9">
-        <v>0.5525563455973117</v>
+        <v>0.54193040342855758</v>
       </c>
       <c r="Q78" s="7">
-        <v>10183803.52</v>
+        <v>10425649.630000001</v>
       </c>
       <c r="R78" s="7">
         <v>0</v>
@@ -36983,7 +36987,7 @@
         <v>4651203.96</v>
       </c>
       <c r="AC78" s="7">
-        <v>244289</v>
+        <v>2442.89</v>
       </c>
       <c r="AD78" s="7">
         <v>223327.48</v>
@@ -37204,19 +37208,19 @@
         <v>161</v>
       </c>
       <c r="M79" s="7">
-        <v>22715176.68</v>
+        <v>1834508.63</v>
       </c>
       <c r="N79" s="4">
         <v>0</v>
       </c>
       <c r="O79" s="7">
-        <v>22821109.760000002</v>
+        <v>1940441.71</v>
       </c>
       <c r="P79" s="9">
-        <v>0.82269681674122563</v>
+        <v>6.995256736756085E-2</v>
       </c>
       <c r="Q79" s="7">
-        <v>4918282.5599999996</v>
+        <v>25798950.609999999</v>
       </c>
       <c r="R79" s="7">
         <v>0</v>
@@ -37384,10 +37388,10 @@
         <v>1423937.02</v>
       </c>
       <c r="BU79" s="7">
-        <v>197.66</v>
+        <v>197661.19</v>
       </c>
       <c r="BV79" s="7">
-        <v>21291042</v>
+        <v>212910.42</v>
       </c>
       <c r="BW79" s="7">
         <v>0</v>
@@ -37477,13 +37481,13 @@
         <v>0</v>
       </c>
       <c r="O80" s="7">
-        <v>5260332.26</v>
+        <v>4991166.83</v>
       </c>
       <c r="P80" s="9">
-        <v>0.99016424125098834</v>
+        <v>0.93949862345464297</v>
       </c>
       <c r="Q80" s="7">
-        <v>52253.31</v>
+        <v>321418.74</v>
       </c>
       <c r="R80" s="7">
         <v>0</v>
@@ -37564,7 +37568,7 @@
         <v>0</v>
       </c>
       <c r="AR80" s="7">
-        <v>299072.7</v>
+        <v>29907.27</v>
       </c>
       <c r="AS80" s="7">
         <v>361569.46</v>
@@ -37746,13 +37750,13 @@
         <v>0</v>
       </c>
       <c r="O81" s="7">
-        <v>5319860.7</v>
+        <v>5316529.71</v>
       </c>
       <c r="P81" s="9">
-        <v>0.99224358916825706</v>
+        <v>0.99162230345055324</v>
       </c>
       <c r="Q81" s="7">
-        <v>41585.58</v>
+        <v>44916.57</v>
       </c>
       <c r="R81" s="7">
         <v>0</v>
@@ -37842,13 +37846,13 @@
         <v>3981.23</v>
       </c>
       <c r="AU81" s="7">
-        <v>1726.3</v>
+        <v>172.63</v>
       </c>
       <c r="AV81" s="7">
         <v>2318.7399999999998</v>
       </c>
       <c r="AW81" s="7">
-        <v>1974.8</v>
+        <v>197.48</v>
       </c>
       <c r="AX81" s="7">
         <v>1382.36</v>
@@ -38549,13 +38553,13 @@
         <v>0</v>
       </c>
       <c r="O84" s="7">
-        <v>235575326.50999999</v>
+        <v>7148655.6200000001</v>
       </c>
       <c r="P84" s="9">
-        <v>32.921240907379328</v>
+        <v>0.99901215172430646</v>
       </c>
       <c r="Q84" s="7">
-        <v>-228419602.12</v>
+        <v>7068.77</v>
       </c>
       <c r="R84" s="7">
         <v>0</v>
@@ -38666,7 +38670,7 @@
         <v>0</v>
       </c>
       <c r="BB84" s="7">
-        <v>3588073</v>
+        <v>35880.730000000003</v>
       </c>
       <c r="BC84" s="7">
         <v>410567.26</v>
@@ -38675,10 +38679,10 @@
         <v>580875.23</v>
       </c>
       <c r="BE84" s="7">
-        <v>106896785</v>
+        <v>1068967.8500000001</v>
       </c>
       <c r="BF84" s="7">
-        <v>120249153</v>
+        <v>1202491.53</v>
       </c>
       <c r="BG84" s="7">
         <v>1185249.6100000001</v>
@@ -39619,13 +39623,13 @@
         <v>0</v>
       </c>
       <c r="O88" s="7">
-        <v>1923627.24</v>
+        <v>1696089.15</v>
       </c>
       <c r="P88" s="9">
-        <v>1.000000005198513</v>
+        <v>0.88171404706097856</v>
       </c>
       <c r="Q88" s="7">
-        <v>-0.01</v>
+        <v>227538.08</v>
       </c>
       <c r="R88" s="7">
         <v>0</v>
@@ -39712,7 +39716,7 @@
         <v>132786.18</v>
       </c>
       <c r="AT88" s="7">
-        <v>170182.8</v>
+        <v>17018.28</v>
       </c>
       <c r="AU88" s="7">
         <v>136974.88</v>
@@ -39757,7 +39761,7 @@
         <v>79200.210000000006</v>
       </c>
       <c r="BI88" s="7">
-        <v>82637.3</v>
+        <v>8263.73</v>
       </c>
       <c r="BJ88" s="7">
         <v>113915.66</v>
@@ -40426,13 +40430,13 @@
         <v>0</v>
       </c>
       <c r="O91" s="7">
-        <v>30456294.329999998</v>
+        <v>29632883.07</v>
       </c>
       <c r="P91" s="9">
-        <v>0.99530376847551394</v>
+        <v>0.96839490289905072</v>
       </c>
       <c r="Q91" s="7">
-        <v>143704.68</v>
+        <v>967115.94</v>
       </c>
       <c r="R91" s="7">
         <v>0</v>
@@ -40522,7 +40526,7 @@
         <v>1414040.86</v>
       </c>
       <c r="AU91" s="7">
-        <v>914901.4</v>
+        <v>91490.14</v>
       </c>
       <c r="AV91" s="7">
         <v>118615.88</v>
@@ -40962,13 +40966,13 @@
         <v>0</v>
       </c>
       <c r="O93" s="7">
-        <v>26930984.010000002</v>
+        <v>25241861.489999998</v>
       </c>
       <c r="P93" s="9">
-        <v>0.99941679870361688</v>
+        <v>0.93673296134625383</v>
       </c>
       <c r="Q93" s="7">
-        <v>15715.35</v>
+        <v>1704837.87</v>
       </c>
       <c r="R93" s="7">
         <v>0</v>
@@ -41064,7 +41068,7 @@
         <v>2020437.14</v>
       </c>
       <c r="AW93" s="7">
-        <v>890788.2</v>
+        <v>89078.82</v>
       </c>
       <c r="AX93" s="7">
         <v>274255.71999999997</v>
@@ -41097,7 +41101,7 @@
         <v>1445406.25</v>
       </c>
       <c r="BH93" s="7">
-        <v>986014.6</v>
+        <v>98601.46</v>
       </c>
       <c r="BI93" s="7">
         <v>1196482.33</v>
@@ -41500,13 +41504,13 @@
         <v>0</v>
       </c>
       <c r="O95" s="7">
-        <v>3538001.16</v>
+        <v>2921910.03</v>
       </c>
       <c r="P95" s="9">
-        <v>0.99126015065260975</v>
+        <v>0.81864670065036704</v>
       </c>
       <c r="Q95" s="7">
-        <v>31194.23</v>
+        <v>647285.36</v>
       </c>
       <c r="R95" s="7">
         <v>0</v>
@@ -41557,7 +41561,7 @@
         <v>347400.67</v>
       </c>
       <c r="AH95" s="7">
-        <v>645282.19999999995</v>
+        <v>64528.22</v>
       </c>
       <c r="AI95" s="7">
         <v>510653.43</v>
@@ -41572,7 +41576,7 @@
         <v>903704.06</v>
       </c>
       <c r="AM95" s="7">
-        <v>39263.5</v>
+        <v>3926.35</v>
       </c>
       <c r="AN95" s="7">
         <v>0</v>
@@ -42034,13 +42038,13 @@
         <v>0</v>
       </c>
       <c r="O97" s="7">
-        <v>724764.22</v>
+        <v>633410.98</v>
       </c>
       <c r="P97" s="9">
         <v>0</v>
       </c>
       <c r="Q97" s="7">
-        <v>-724764.22</v>
+        <v>-633410.98</v>
       </c>
       <c r="R97" s="7">
         <v>0</v>
@@ -42130,7 +42134,7 @@
         <v>114920.76</v>
       </c>
       <c r="AU97" s="7">
-        <v>101503.6</v>
+        <v>10150.36</v>
       </c>
       <c r="AV97" s="7">
         <v>0</v>
@@ -42831,19 +42835,19 @@
         <v>396</v>
       </c>
       <c r="M100" s="7">
-        <v>38656978.789999999</v>
+        <v>1612016.33</v>
       </c>
       <c r="N100" s="4">
         <v>0</v>
       </c>
       <c r="O100" s="7">
-        <v>38656978.789999999</v>
+        <v>1612016.33</v>
       </c>
       <c r="P100" s="9">
-        <v>23.978455956175871</v>
+        <v>0.99991421418428095</v>
       </c>
       <c r="Q100" s="7">
-        <v>-37044824.159999996</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="R100" s="7">
         <v>0</v>
@@ -43014,7 +43018,7 @@
         <v>233380.03</v>
       </c>
       <c r="BV100" s="7">
-        <v>37419154</v>
+        <v>374191.54</v>
       </c>
       <c r="BW100" s="7">
         <v>51750.66</v>
@@ -43100,19 +43104,19 @@
         <v>398</v>
       </c>
       <c r="M101" s="7">
-        <v>309189045.25</v>
+        <v>21884193.460000001</v>
       </c>
       <c r="N101" s="4">
         <v>0</v>
       </c>
       <c r="O101" s="7">
-        <v>312407129.72000003</v>
+        <v>25102277.93</v>
       </c>
       <c r="P101" s="9">
-        <v>12.407049386845079</v>
+        <v>0.99692091623824075</v>
       </c>
       <c r="Q101" s="7">
-        <v>-287227321.05000001</v>
+        <v>77530.740000000005</v>
       </c>
       <c r="R101" s="7">
         <v>0</v>
@@ -43280,10 +43284,10 @@
         <v>3472953.84</v>
       </c>
       <c r="BU101" s="7">
-        <v>46161782</v>
+        <v>461617.82</v>
       </c>
       <c r="BV101" s="7">
-        <v>244045139</v>
+        <v>2440451.39</v>
       </c>
       <c r="BW101" s="7">
         <v>0</v>
@@ -44989,13 +44993,13 @@
         <v>0</v>
       </c>
       <c r="O108" s="7">
-        <v>13048536.539999999</v>
+        <v>12688117.140000001</v>
       </c>
       <c r="P108" s="9">
-        <v>0.7730065769207074</v>
+        <v>0.75165502030776821</v>
       </c>
       <c r="Q108" s="7">
-        <v>3831703.46</v>
+        <v>4192122.86</v>
       </c>
       <c r="R108" s="7">
         <v>0</v>
@@ -45055,10 +45059,10 @@
         <v>679932.12</v>
       </c>
       <c r="AK108" s="7">
-        <v>194089.8</v>
+        <v>19408.98</v>
       </c>
       <c r="AL108" s="7">
-        <v>206376.2</v>
+        <v>20637.62</v>
       </c>
       <c r="AM108" s="7">
         <v>0</v>
@@ -45796,13 +45800,13 @@
         <v>0</v>
       </c>
       <c r="O111" s="7">
-        <v>8398407.2300000004</v>
+        <v>7956304.1900000004</v>
       </c>
       <c r="P111" s="9">
-        <v>0.34753819686225279</v>
+        <v>0.3292433358081146</v>
       </c>
       <c r="Q111" s="7">
-        <v>15767014.890000001</v>
+        <v>16209117.93</v>
       </c>
       <c r="R111" s="7">
         <v>0</v>
@@ -45844,7 +45848,7 @@
         <v>85270.45</v>
       </c>
       <c r="AE111" s="7">
-        <v>183497.2</v>
+        <v>18349.72</v>
       </c>
       <c r="AF111" s="7">
         <v>269577.71999999997</v>
@@ -45853,7 +45857,7 @@
         <v>270437.77</v>
       </c>
       <c r="AH111" s="7">
-        <v>273799.2</v>
+        <v>27379.919999999998</v>
       </c>
       <c r="AI111" s="7">
         <v>371021.51</v>
@@ -45901,7 +45905,7 @@
         <v>133423.93</v>
       </c>
       <c r="AX111" s="7">
-        <v>33929.199999999997</v>
+        <v>3392.92</v>
       </c>
       <c r="AY111" s="7">
         <v>1505821.47</v>
@@ -46065,13 +46069,13 @@
         <v>0</v>
       </c>
       <c r="O112" s="7">
-        <v>653661.5</v>
+        <v>242119.4</v>
       </c>
       <c r="P112" s="9">
-        <v>0.18077641169436459</v>
+        <v>6.6960462461981521E-2</v>
       </c>
       <c r="Q112" s="7">
-        <v>2962194.65</v>
+        <v>3373736.75</v>
       </c>
       <c r="R112" s="7">
         <v>0</v>
@@ -46173,10 +46177,10 @@
         <v>6051.68</v>
       </c>
       <c r="AY112" s="7">
-        <v>15072.3</v>
+        <v>1507.23</v>
       </c>
       <c r="AZ112" s="7">
-        <v>401997</v>
+        <v>4019.97</v>
       </c>
       <c r="BA112" s="7">
         <v>0</v>
@@ -46334,13 +46338,13 @@
         <v>0</v>
       </c>
       <c r="O113" s="7">
-        <v>14985593.439999999</v>
+        <v>12874385.859999999</v>
       </c>
       <c r="P113" s="9">
-        <v>0.99936673668141041</v>
+        <v>0.85857347159456188</v>
       </c>
       <c r="Q113" s="7">
-        <v>9495.84</v>
+        <v>2120703.42</v>
       </c>
       <c r="R113" s="7">
         <v>0</v>
@@ -46394,7 +46398,7 @@
         <v>0</v>
       </c>
       <c r="AI113" s="7">
-        <v>906377.1</v>
+        <v>90637.71</v>
       </c>
       <c r="AJ113" s="7">
         <v>0</v>
@@ -46409,7 +46413,7 @@
         <v>1077897.6200000001</v>
       </c>
       <c r="AN113" s="7">
-        <v>966233.59999999998</v>
+        <v>96623.360000000001</v>
       </c>
       <c r="AO113" s="7">
         <v>0</v>
@@ -46457,7 +46461,7 @@
         <v>60941.37</v>
       </c>
       <c r="BD113" s="7">
-        <v>473175.5</v>
+        <v>47317.55</v>
       </c>
       <c r="BE113" s="7">
         <v>1022166.32</v>
@@ -46866,19 +46870,19 @@
         <v>161</v>
       </c>
       <c r="M115" s="7">
-        <v>25290453.199999999</v>
+        <v>1082086.6299999999</v>
       </c>
       <c r="N115" s="4">
         <v>0</v>
       </c>
       <c r="O115" s="7">
-        <v>46134005.090000004</v>
+        <v>20224500.370000001</v>
       </c>
       <c r="P115" s="9">
-        <v>1.876063233884028</v>
+        <v>0.82243979237899134</v>
       </c>
       <c r="Q115" s="7">
-        <v>-21543146.82</v>
+        <v>4366357.9000000004</v>
       </c>
       <c r="R115" s="7">
         <v>0</v>
@@ -46923,10 +46927,10 @@
         <v>0</v>
       </c>
       <c r="AF115" s="7">
-        <v>821885</v>
+        <v>8218.85</v>
       </c>
       <c r="AG115" s="7">
-        <v>666034.69999999995</v>
+        <v>66603.47</v>
       </c>
       <c r="AH115" s="7">
         <v>1095907.96</v>
@@ -46986,7 +46990,7 @@
         <v>1471882.58</v>
       </c>
       <c r="BA115" s="7">
-        <v>320045.3</v>
+        <v>32004.53</v>
       </c>
       <c r="BB115" s="7">
         <v>106063.07</v>
@@ -47040,13 +47044,13 @@
         <v>80543.75</v>
       </c>
       <c r="BS115" s="7">
-        <v>93.14</v>
+        <v>93138.76</v>
       </c>
       <c r="BT115" s="7">
         <v>498838.01</v>
       </c>
       <c r="BU115" s="7">
-        <v>24546881</v>
+        <v>245468.81</v>
       </c>
       <c r="BV115" s="7">
         <v>0</v>
@@ -47373,6 +47377,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
chore: update BASE.xlsx data
</commit_message>
<xml_diff>
--- a/MEDIÇÕES_CONSOLIDADO.xlsx
+++ b/MEDIÇÕES_CONSOLIDADO.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
-  <workbookPr codeName="EstaPastaDeTrabalho"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDICOES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAF4932-6DD1-438F-AC8E-C2F6A70CE9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3622BA-9575-4876-9CD9-68494AFD448D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,9 @@
     <sheet name="PROBLEMAS" sheetId="2" r:id="rId2"/>
     <sheet name="GESTOR_FALTANTES" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Medições!$A$1:$CK$49</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1568,7 +1571,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{A2B6AE1F-0AB3-49E3-8F97-AA27B0F5E824}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{FA7612CA-BB5F-4472-8802-45E6C239BFB6}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1866,12 +1869,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:CK49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:CK1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1884,12 +1884,12 @@
     <col min="8" max="8" width="10.5703125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="8.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="11" max="11" width="22" customWidth="1"/>
     <col min="12" max="12" width="18.28515625" customWidth="1"/>
     <col min="13" max="15" width="18" customWidth="1"/>
     <col min="16" max="16" width="8" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="18" max="89" width="20" hidden="1" customWidth="1"/>
+    <col min="18" max="89" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:89" ht="30" x14ac:dyDescent="0.25">
@@ -3281,13 +3281,13 @@
         <v>0</v>
       </c>
       <c r="O6" s="6">
-        <v>7070321.0300000003</v>
+        <v>7322834.1200000001</v>
       </c>
       <c r="P6" s="8">
-        <v>0.83535114997594728</v>
+        <v>0.86518531156782619</v>
       </c>
       <c r="Q6" s="6">
-        <v>1393569.91</v>
+        <v>1141056.82</v>
       </c>
       <c r="R6" s="6">
         <v>0</v>
@@ -3347,7 +3347,7 @@
         <v>251528.78</v>
       </c>
       <c r="AK6" s="6">
-        <v>28057.01</v>
+        <v>280570.09999999998</v>
       </c>
       <c r="AL6" s="6">
         <v>241160.41</v>
@@ -3550,13 +3550,13 @@
         <v>0</v>
       </c>
       <c r="O7" s="6">
-        <v>1145901.75</v>
+        <v>1222003.4099999999</v>
       </c>
       <c r="P7" s="8">
-        <v>0.74950227898642985</v>
+        <v>0.799278245909118</v>
       </c>
       <c r="Q7" s="6">
-        <v>382981.86</v>
+        <v>306880.2</v>
       </c>
       <c r="R7" s="6">
         <v>0</v>
@@ -3676,7 +3676,7 @@
         <v>0</v>
       </c>
       <c r="BE7" s="6">
-        <v>8455.74</v>
+        <v>84557.4</v>
       </c>
       <c r="BF7" s="6">
         <v>123108.53</v>
@@ -3813,19 +3813,19 @@
         <v>117</v>
       </c>
       <c r="M8" s="6">
-        <v>579644.25</v>
+        <v>730910.4</v>
       </c>
       <c r="N8" s="6">
         <v>0</v>
       </c>
       <c r="O8" s="6">
-        <v>887614.06</v>
+        <v>1038880.21</v>
       </c>
       <c r="P8" s="8">
-        <v>0.26941498255451801</v>
+        <v>0.31532836878832671</v>
       </c>
       <c r="Q8" s="6">
-        <v>2406983.9300000002</v>
+        <v>2255717.7799999998</v>
       </c>
       <c r="R8" s="6">
         <v>0</v>
@@ -3990,7 +3990,7 @@
         <v>224011.87</v>
       </c>
       <c r="BT8" s="6">
-        <v>16807.349999999999</v>
+        <v>168073.5</v>
       </c>
       <c r="BU8" s="6">
         <v>300274.31</v>
@@ -4351,19 +4351,19 @@
         <v>122</v>
       </c>
       <c r="M10" s="6">
-        <v>8583843.9700000007</v>
+        <v>8765166.1600000001</v>
       </c>
       <c r="N10" s="6">
         <v>0</v>
       </c>
       <c r="O10" s="6">
-        <v>53244971.829999998</v>
+        <v>54515037.340000004</v>
       </c>
       <c r="P10" s="8">
-        <v>0.94759670100333215</v>
+        <v>0.97019995997728137</v>
       </c>
       <c r="Q10" s="6">
-        <v>2944514.45</v>
+        <v>1674448.94</v>
       </c>
       <c r="R10" s="6">
         <v>0</v>
@@ -4447,16 +4447,16 @@
         <v>0</v>
       </c>
       <c r="AS10" s="6">
-        <v>82087.149999999994</v>
+        <v>820871.5</v>
       </c>
       <c r="AT10" s="6">
-        <v>17911.55</v>
+        <v>179115.5</v>
       </c>
       <c r="AU10" s="6">
         <v>2750605.37</v>
       </c>
       <c r="AV10" s="6">
-        <v>20972.78</v>
+        <v>209727.8</v>
       </c>
       <c r="AW10" s="6">
         <v>195003.86</v>
@@ -4531,7 +4531,7 @@
         <v>206718.42</v>
       </c>
       <c r="BU10" s="6">
-        <v>20146.91</v>
+        <v>201469.1</v>
       </c>
       <c r="BV10" s="6">
         <v>205661.78</v>
@@ -5423,19 +5423,19 @@
         <v>130</v>
       </c>
       <c r="M14" s="6">
-        <v>842876.36</v>
+        <v>0</v>
       </c>
       <c r="N14" s="6">
         <v>0</v>
       </c>
       <c r="O14" s="6">
-        <v>842876.36</v>
+        <v>0</v>
       </c>
       <c r="P14" s="8">
-        <v>0.1073998805403075</v>
+        <v>0</v>
       </c>
       <c r="Q14" s="6">
-        <v>7005143.1699999999</v>
+        <v>7848019.5300000003</v>
       </c>
       <c r="R14" s="6">
         <v>0</v>
@@ -5615,7 +5615,7 @@
         <v>0</v>
       </c>
       <c r="BY14" s="6">
-        <v>842876.36</v>
+        <v>0</v>
       </c>
       <c r="BZ14" s="6">
         <v>0</v>
@@ -5692,19 +5692,19 @@
         <v>135</v>
       </c>
       <c r="M15" s="6">
-        <v>10045837.32</v>
+        <v>10584628.26</v>
       </c>
       <c r="N15" s="6">
         <v>0</v>
       </c>
       <c r="O15" s="6">
-        <v>31523514.969999999</v>
+        <v>32294745.039999999</v>
       </c>
       <c r="P15" s="8">
-        <v>0.6450147068705594</v>
+        <v>0.66079514055646738</v>
       </c>
       <c r="Q15" s="6">
-        <v>17349037.289999999</v>
+        <v>16577807.220000001</v>
       </c>
       <c r="R15" s="6">
         <v>0</v>
@@ -5800,7 +5800,7 @@
         <v>604692.32999999996</v>
       </c>
       <c r="AW15" s="6">
-        <v>2347.87</v>
+        <v>234787</v>
       </c>
       <c r="AX15" s="6">
         <v>435109.34</v>
@@ -5878,7 +5878,7 @@
         <v>762624.41</v>
       </c>
       <c r="BW15" s="6">
-        <v>59865.66</v>
+        <v>598656.6</v>
       </c>
       <c r="BX15" s="6">
         <v>314589.38</v>
@@ -6230,13 +6230,13 @@
         <v>0</v>
       </c>
       <c r="O17" s="6">
-        <v>29693198.199999999</v>
+        <v>29783885.440000001</v>
       </c>
       <c r="P17" s="8">
-        <v>0.85662541443485507</v>
+        <v>0.85924166998354001</v>
       </c>
       <c r="Q17" s="6">
-        <v>4969791.83</v>
+        <v>4879104.59</v>
       </c>
       <c r="R17" s="6">
         <v>0</v>
@@ -6332,7 +6332,7 @@
         <v>0</v>
       </c>
       <c r="AW17" s="6">
-        <v>10076.36</v>
+        <v>100763.6</v>
       </c>
       <c r="AX17" s="6">
         <v>104212.78</v>
@@ -6768,13 +6768,13 @@
         <v>0</v>
       </c>
       <c r="O19" s="6">
-        <v>28612913.760000002</v>
+        <v>29153437.02</v>
       </c>
       <c r="P19" s="8">
-        <v>0.43565081298788411</v>
+        <v>0.44388064234511138</v>
       </c>
       <c r="Q19" s="6">
-        <v>37065636.369999997</v>
+        <v>36525113.109999999</v>
       </c>
       <c r="R19" s="6">
         <v>0</v>
@@ -6843,7 +6843,7 @@
         <v>967768.24</v>
       </c>
       <c r="AN19" s="6">
-        <v>54045.29</v>
+        <v>540452.9</v>
       </c>
       <c r="AO19" s="6">
         <v>609973.01</v>
@@ -6882,7 +6882,7 @@
         <v>273099.03000000003</v>
       </c>
       <c r="BA19" s="6">
-        <v>6012.85</v>
+        <v>60128.5</v>
       </c>
       <c r="BB19" s="6">
         <v>508655.35999999999</v>
@@ -7031,19 +7031,19 @@
         <v>149</v>
       </c>
       <c r="M20" s="6">
-        <v>8177086.2000000002</v>
+        <v>9076344.5099999998</v>
       </c>
       <c r="N20" s="6">
         <v>0</v>
       </c>
       <c r="O20" s="6">
-        <v>21095002.079999998</v>
+        <v>22442987.52</v>
       </c>
       <c r="P20" s="8">
-        <v>0.36350379828114149</v>
+        <v>0.38673194614334239</v>
       </c>
       <c r="Q20" s="6">
-        <v>36937409.630000003</v>
+        <v>35589424.189999998</v>
       </c>
       <c r="R20" s="6">
         <v>0</v>
@@ -7151,7 +7151,7 @@
         <v>444020.59</v>
       </c>
       <c r="BA20" s="6">
-        <v>49858.57</v>
+        <v>498585.7</v>
       </c>
       <c r="BB20" s="6">
         <v>357750.39</v>
@@ -7211,7 +7211,7 @@
         <v>1607390.05</v>
       </c>
       <c r="BU20" s="6">
-        <v>99917.59</v>
+        <v>999175.9</v>
       </c>
       <c r="BV20" s="6">
         <v>1290254.3700000001</v>
@@ -7569,19 +7569,19 @@
         <v>151</v>
       </c>
       <c r="M22" s="6">
-        <v>22867981.510000002</v>
+        <v>23400418.18</v>
       </c>
       <c r="N22" s="6">
         <v>0</v>
       </c>
       <c r="O22" s="6">
-        <v>35263725.240000002</v>
+        <v>35796161.909999996</v>
       </c>
       <c r="P22" s="8">
-        <v>0.76890258227510955</v>
+        <v>0.78051201740071507</v>
       </c>
       <c r="Q22" s="6">
-        <v>10598684.449999999</v>
+        <v>10066247.779999999</v>
       </c>
       <c r="R22" s="6">
         <v>0</v>
@@ -7734,7 +7734,7 @@
         <v>1505339.86</v>
       </c>
       <c r="BP22" s="6">
-        <v>59159.63</v>
+        <v>591596.30000000005</v>
       </c>
       <c r="BQ22" s="6">
         <v>762847.31</v>
@@ -8107,19 +8107,19 @@
         <v>159</v>
       </c>
       <c r="M24" s="6">
-        <v>33128534.579999998</v>
+        <v>33221220.629999999</v>
       </c>
       <c r="N24" s="6">
         <v>0</v>
       </c>
       <c r="O24" s="6">
-        <v>45358734.43</v>
+        <v>45451420.479999997</v>
       </c>
       <c r="P24" s="8">
-        <v>0.88221205578748352</v>
+        <v>0.88401476813695412</v>
       </c>
       <c r="Q24" s="6">
-        <v>6056040.6600000001</v>
+        <v>5963354.6100000003</v>
       </c>
       <c r="R24" s="6">
         <v>0</v>
@@ -8296,7 +8296,7 @@
         <v>970563.95</v>
       </c>
       <c r="BX24" s="6">
-        <v>10298.450000000001</v>
+        <v>102984.5</v>
       </c>
       <c r="BY24" s="6">
         <v>3383264.9</v>
@@ -8376,19 +8376,19 @@
         <v>162</v>
       </c>
       <c r="M25" s="6">
-        <v>2106573.67</v>
+        <v>2286082.54</v>
       </c>
       <c r="N25" s="6">
         <v>0</v>
       </c>
       <c r="O25" s="6">
-        <v>2106573.67</v>
+        <v>2286082.54</v>
       </c>
       <c r="P25" s="8">
-        <v>0.80962546794254309</v>
+        <v>0.87861662402852381</v>
       </c>
       <c r="Q25" s="6">
-        <v>495337.65</v>
+        <v>315828.78000000003</v>
       </c>
       <c r="R25" s="6">
         <v>0</v>
@@ -8565,7 +8565,7 @@
         <v>126570.92</v>
       </c>
       <c r="BX25" s="6">
-        <v>19945.43</v>
+        <v>199454.3</v>
       </c>
       <c r="BY25" s="6">
         <v>129958.08</v>
@@ -8914,19 +8914,19 @@
         <v>167</v>
       </c>
       <c r="M27" s="6">
-        <v>18958744.699999999</v>
+        <v>19557304.370000001</v>
       </c>
       <c r="N27" s="6">
         <v>0</v>
       </c>
       <c r="O27" s="6">
-        <v>19246406.859999999</v>
+        <v>19844966.530000001</v>
       </c>
       <c r="P27" s="8">
-        <v>0.67626506067349024</v>
+        <v>0.69729677815165103</v>
       </c>
       <c r="Q27" s="6">
-        <v>9213450.0500000007</v>
+        <v>8614890.3800000008</v>
       </c>
       <c r="R27" s="6">
         <v>0</v>
@@ -9085,7 +9085,7 @@
         <v>133461.04</v>
       </c>
       <c r="BR27" s="6">
-        <v>66506.63</v>
+        <v>665066.30000000005</v>
       </c>
       <c r="BS27" s="6">
         <v>1225871.8</v>
@@ -9183,19 +9183,19 @@
         <v>167</v>
       </c>
       <c r="M28" s="6">
-        <v>3976099.14</v>
+        <v>5250302.04</v>
       </c>
       <c r="N28" s="6">
-        <v>0</v>
+        <v>499862.54</v>
       </c>
       <c r="O28" s="6">
-        <v>32751450.57</v>
+        <v>36377601.259999998</v>
       </c>
       <c r="P28" s="8">
-        <v>0.71625177422331798</v>
+        <v>0.79555320423975362</v>
       </c>
       <c r="Q28" s="6">
-        <v>12974719.68</v>
+        <v>9348568.9900000002</v>
       </c>
       <c r="R28" s="6">
         <v>0</v>
@@ -9282,13 +9282,13 @@
         <v>654423.03</v>
       </c>
       <c r="AT28" s="6">
-        <v>84745.84</v>
+        <v>847458.4</v>
       </c>
       <c r="AU28" s="6">
-        <v>99642.880000000005</v>
+        <v>996428.80000000005</v>
       </c>
       <c r="AV28" s="6">
-        <v>21398.53</v>
+        <v>213985.3</v>
       </c>
       <c r="AW28" s="6">
         <v>122099.63</v>
@@ -9363,7 +9363,7 @@
         <v>289529.71000000002</v>
       </c>
       <c r="BU28" s="6">
-        <v>53264.68</v>
+        <v>532646.80000000005</v>
       </c>
       <c r="BV28" s="6">
         <v>485170.46</v>
@@ -9372,13 +9372,13 @@
         <v>1012783.71</v>
       </c>
       <c r="BX28" s="6">
-        <v>88313.42</v>
+        <v>883134.2</v>
       </c>
       <c r="BY28" s="6">
         <v>837187.79</v>
       </c>
       <c r="BZ28" s="6">
-        <v>0</v>
+        <v>499862.54</v>
       </c>
       <c r="CA28" s="6">
         <v>0</v>
@@ -9452,19 +9452,19 @@
         <v>167</v>
       </c>
       <c r="M29" s="6">
-        <v>8061194.3200000003</v>
+        <v>8362397.1399999997</v>
       </c>
       <c r="N29" s="6">
         <v>0</v>
       </c>
       <c r="O29" s="6">
-        <v>39541097.210000001</v>
+        <v>42048979.520000003</v>
       </c>
       <c r="P29" s="8">
-        <v>0.90282754196168558</v>
+        <v>0.96008910982970819</v>
       </c>
       <c r="Q29" s="6">
-        <v>4255857.7699999996</v>
+        <v>1747975.46</v>
       </c>
       <c r="R29" s="6">
         <v>0</v>
@@ -9536,7 +9536,7 @@
         <v>904885.44</v>
       </c>
       <c r="AO29" s="6">
-        <v>72723.34</v>
+        <v>727233.4</v>
       </c>
       <c r="AP29" s="6">
         <v>0</v>
@@ -9560,7 +9560,7 @@
         <v>536795.13</v>
       </c>
       <c r="AW29" s="6">
-        <v>60647.07</v>
+        <v>606470.69999999995</v>
       </c>
       <c r="AX29" s="6">
         <v>608799.93999999994</v>
@@ -9575,10 +9575,10 @@
         <v>289836.99</v>
       </c>
       <c r="BB29" s="6">
-        <v>65030.65</v>
+        <v>650306.5</v>
       </c>
       <c r="BC29" s="6">
-        <v>46785.55</v>
+        <v>467855.5</v>
       </c>
       <c r="BD29" s="6">
         <v>951169.12</v>
@@ -9644,7 +9644,7 @@
         <v>210535.57</v>
       </c>
       <c r="BY29" s="6">
-        <v>33466.980000000003</v>
+        <v>334669.8</v>
       </c>
       <c r="BZ29" s="6">
         <v>0</v>
@@ -9721,19 +9721,19 @@
         <v>171</v>
       </c>
       <c r="M30" s="6">
-        <v>2362289.83</v>
+        <v>2715707.77</v>
       </c>
       <c r="N30" s="6">
         <v>0</v>
       </c>
       <c r="O30" s="6">
-        <v>12761723.09</v>
+        <v>13115141.029999999</v>
       </c>
       <c r="P30" s="8">
-        <v>0.55910817423144876</v>
+        <v>0.57459188734608901</v>
       </c>
       <c r="Q30" s="6">
-        <v>10063418.23</v>
+        <v>9710000.2899999991</v>
       </c>
       <c r="R30" s="6">
         <v>0</v>
@@ -9913,7 +9913,7 @@
         <v>367117.37</v>
       </c>
       <c r="BY30" s="6">
-        <v>39268.660000000003</v>
+        <v>392686.6</v>
       </c>
       <c r="BZ30" s="6">
         <v>0</v>
@@ -9990,19 +9990,19 @@
         <v>171</v>
       </c>
       <c r="M31" s="6">
-        <v>3085620.1</v>
+        <v>3253833.79</v>
       </c>
       <c r="N31" s="6">
         <v>0</v>
       </c>
       <c r="O31" s="6">
-        <v>14180497.4</v>
+        <v>14348711.09</v>
       </c>
       <c r="P31" s="8">
-        <v>0.5350265223567584</v>
+        <v>0.54137318164767279</v>
       </c>
       <c r="Q31" s="6">
-        <v>12323791.279999999</v>
+        <v>12155577.59</v>
       </c>
       <c r="R31" s="6">
         <v>0</v>
@@ -10149,7 +10149,7 @@
         <v>0</v>
       </c>
       <c r="BN31" s="6">
-        <v>18690.41</v>
+        <v>186904.1</v>
       </c>
       <c r="BO31" s="6">
         <v>1214701.27</v>
@@ -10265,13 +10265,13 @@
         <v>0</v>
       </c>
       <c r="O32" s="6">
-        <v>14156092.16</v>
+        <v>15889085.539999999</v>
       </c>
       <c r="P32" s="8">
-        <v>0.70407202192505791</v>
+        <v>0.7902647465307262</v>
       </c>
       <c r="Q32" s="6">
-        <v>5949936.3700000001</v>
+        <v>4216942.99</v>
       </c>
       <c r="R32" s="6">
         <v>0</v>
@@ -10391,7 +10391,7 @@
         <v>0</v>
       </c>
       <c r="BE32" s="6">
-        <v>53124.32</v>
+        <v>531243.19999999995</v>
       </c>
       <c r="BF32" s="6">
         <v>111606.91</v>
@@ -10406,13 +10406,13 @@
         <v>751552.98</v>
       </c>
       <c r="BJ32" s="6">
-        <v>80.5</v>
+        <v>805000</v>
       </c>
       <c r="BK32" s="6">
         <v>630821.07999999996</v>
       </c>
       <c r="BL32" s="6">
-        <v>45</v>
+        <v>450000</v>
       </c>
       <c r="BM32" s="6">
         <v>0</v>
@@ -10534,13 +10534,13 @@
         <v>0</v>
       </c>
       <c r="O33" s="6">
-        <v>6142640.3200000003</v>
+        <v>7571952.2800000003</v>
       </c>
       <c r="P33" s="8">
-        <v>0.78795637028039589</v>
+        <v>0.97130349876731303</v>
       </c>
       <c r="Q33" s="6">
-        <v>1653020.14</v>
+        <v>223708.18</v>
       </c>
       <c r="R33" s="6">
         <v>0</v>
@@ -10618,7 +10618,7 @@
         <v>1055071.1200000001</v>
       </c>
       <c r="AQ33" s="6">
-        <v>52306.63</v>
+        <v>523066.3</v>
       </c>
       <c r="AR33" s="6">
         <v>1069722.6100000001</v>
@@ -10648,7 +10648,7 @@
         <v>170056.31</v>
       </c>
       <c r="BA33" s="6">
-        <v>2792.64</v>
+        <v>279264</v>
       </c>
       <c r="BB33" s="6">
         <v>0</v>
@@ -10666,13 +10666,13 @@
         <v>698367.68</v>
       </c>
       <c r="BG33" s="6">
-        <v>67595.02</v>
+        <v>675950.2</v>
       </c>
       <c r="BH33" s="6">
         <v>354120.32</v>
       </c>
       <c r="BI33" s="6">
-        <v>8191.75</v>
+        <v>81917.5</v>
       </c>
       <c r="BJ33" s="6">
         <v>224576.79</v>
@@ -11338,16 +11338,16 @@
         <v>2420969.38</v>
       </c>
       <c r="N36" s="6">
-        <v>0</v>
+        <v>3055826.41</v>
       </c>
       <c r="O36" s="6">
-        <v>2420969.38</v>
+        <v>5476795.79</v>
       </c>
       <c r="P36" s="8">
-        <v>0.23392386008833299</v>
+        <v>0.52919017592545148</v>
       </c>
       <c r="Q36" s="6">
-        <v>7928421.1399999997</v>
+        <v>4872594.7300000004</v>
       </c>
       <c r="R36" s="6">
         <v>0</v>
@@ -11530,7 +11530,7 @@
         <v>2063903.13</v>
       </c>
       <c r="BZ36" s="6">
-        <v>0</v>
+        <v>3055826.41</v>
       </c>
       <c r="CA36" s="6">
         <v>0</v>
@@ -11873,19 +11873,19 @@
         <v>188</v>
       </c>
       <c r="M38" s="6">
-        <v>368496.83</v>
+        <v>548089.31000000006</v>
       </c>
       <c r="N38" s="6">
         <v>0</v>
       </c>
       <c r="O38" s="6">
-        <v>368496.83</v>
+        <v>548089.31000000006</v>
       </c>
       <c r="P38" s="8">
-        <v>0.48277746347115108</v>
+        <v>0.71806633136424369</v>
       </c>
       <c r="Q38" s="6">
-        <v>394788.24</v>
+        <v>215195.76</v>
       </c>
       <c r="R38" s="6">
         <v>0</v>
@@ -12044,7 +12044,7 @@
         <v>0</v>
       </c>
       <c r="BR38" s="6">
-        <v>2193.96</v>
+        <v>21939.599999999999</v>
       </c>
       <c r="BS38" s="6">
         <v>0</v>
@@ -12065,7 +12065,7 @@
         <v>233489.27</v>
       </c>
       <c r="BY38" s="6">
-        <v>17760.759999999998</v>
+        <v>177607.6</v>
       </c>
       <c r="BZ38" s="6">
         <v>0</v>
@@ -12686,13 +12686,13 @@
         <v>0</v>
       </c>
       <c r="O41" s="6">
-        <v>2270712.37</v>
+        <v>2301268.7200000002</v>
       </c>
       <c r="P41" s="8">
-        <v>0.14935474991911379</v>
+        <v>0.15136457559011721</v>
       </c>
       <c r="Q41" s="6">
-        <v>12932770.42</v>
+        <v>12902214.07</v>
       </c>
       <c r="R41" s="6">
         <v>0</v>
@@ -12827,7 +12827,7 @@
         <v>64140.14</v>
       </c>
       <c r="BJ41" s="6">
-        <v>308.64999999999998</v>
+        <v>30865</v>
       </c>
       <c r="BK41" s="6">
         <v>53092.18</v>
@@ -12952,16 +12952,16 @@
         <v>11147804.810000001</v>
       </c>
       <c r="N42" s="6">
-        <v>0</v>
+        <v>1289167.06</v>
       </c>
       <c r="O42" s="6">
-        <v>11147804.810000001</v>
+        <v>12436971.869999999</v>
       </c>
       <c r="P42" s="8">
-        <v>0.46089188035778328</v>
+        <v>0.51419086078536724</v>
       </c>
       <c r="Q42" s="6">
-        <v>13039657.119999999</v>
+        <v>11750490.060000001</v>
       </c>
       <c r="R42" s="6">
         <v>0</v>
@@ -13144,7 +13144,7 @@
         <v>2441141.7799999998</v>
       </c>
       <c r="BZ42" s="6">
-        <v>0</v>
+        <v>1289167.06</v>
       </c>
       <c r="CA42" s="6">
         <v>0</v>
@@ -13762,13 +13762,13 @@
         <v>0</v>
       </c>
       <c r="O45" s="6">
-        <v>55215321.43</v>
+        <v>56075179.539999999</v>
       </c>
       <c r="P45" s="8">
-        <v>0.93350146587305338</v>
+        <v>0.94803871360320446</v>
       </c>
       <c r="Q45" s="6">
-        <v>3933296.38</v>
+        <v>3073438.27</v>
       </c>
       <c r="R45" s="6">
         <v>0</v>
@@ -13888,7 +13888,7 @@
         <v>187923.63</v>
       </c>
       <c r="BE45" s="6">
-        <v>51512.81</v>
+        <v>515128.1</v>
       </c>
       <c r="BF45" s="6">
         <v>142691.85999999999</v>
@@ -13912,7 +13912,7 @@
         <v>1021876.31</v>
       </c>
       <c r="BM45" s="6">
-        <v>44026.98</v>
+        <v>440269.8</v>
       </c>
       <c r="BN45" s="6">
         <v>1729073.23</v>
@@ -14300,13 +14300,13 @@
         <v>0</v>
       </c>
       <c r="O47" s="6">
-        <v>38672688.490000002</v>
+        <v>38738669.020000003</v>
       </c>
       <c r="P47" s="8">
-        <v>0.92848793103789606</v>
+        <v>0.93007204965443158</v>
       </c>
       <c r="Q47" s="6">
-        <v>2978567.49</v>
+        <v>2912586.96</v>
       </c>
       <c r="R47" s="6">
         <v>0</v>
@@ -14426,7 +14426,7 @@
         <v>0</v>
       </c>
       <c r="BE47" s="6">
-        <v>666.47</v>
+        <v>66647</v>
       </c>
       <c r="BF47" s="6">
         <v>7823810.8099999996</v>
@@ -14832,19 +14832,19 @@
         <v>211</v>
       </c>
       <c r="M49" s="6">
-        <v>53528793.799999997</v>
+        <v>55173009.469999999</v>
       </c>
       <c r="N49" s="6">
         <v>0</v>
       </c>
       <c r="O49" s="6">
-        <v>60266935.369999997</v>
+        <v>61911151.039999999</v>
       </c>
       <c r="P49" s="8">
-        <v>0.80776353215789221</v>
+        <v>0.82980111294866332</v>
       </c>
       <c r="Q49" s="6">
-        <v>14342691.050000001</v>
+        <v>12698475.380000001</v>
       </c>
       <c r="R49" s="6">
         <v>0</v>
@@ -14997,7 +14997,7 @@
         <v>380731.29</v>
       </c>
       <c r="BP49" s="6">
-        <v>94172.57</v>
+        <v>941725.7</v>
       </c>
       <c r="BQ49" s="6">
         <v>7173927.79</v>
@@ -15009,7 +15009,7 @@
         <v>911822.65</v>
       </c>
       <c r="BT49" s="6">
-        <v>797.46</v>
+        <v>797460</v>
       </c>
       <c r="BU49" s="6">
         <v>4046951.13</v>
@@ -15064,15 +15064,13 @@
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.15748031496062992" right="0.74803149606299213" top="0.23622047244094491" bottom="0.27559055118110237" header="0.15748031496062992" footer="0.15748031496062992"/>
-  <pageSetup paperSize="8" scale="80" orientation="landscape" r:id="rId1"/>
+  <autoFilter ref="A1:CK49" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:CK127"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15409,13 +15407,13 @@
         <v>0</v>
       </c>
       <c r="O2" s="6">
-        <v>985523.15</v>
+        <v>1088826.01</v>
       </c>
       <c r="P2" s="8">
-        <v>0.81281452368690832</v>
+        <v>0.89801400879935389</v>
       </c>
       <c r="Q2" s="6">
-        <v>226959.06</v>
+        <v>123656.2</v>
       </c>
       <c r="R2" s="6">
         <v>0</v>
@@ -15439,7 +15437,7 @@
         <v>170033.46</v>
       </c>
       <c r="Y2" s="6">
-        <v>0</v>
+        <v>103302.86</v>
       </c>
       <c r="Z2" s="6">
         <v>120559.29</v>
@@ -15676,13 +15674,13 @@
         <v>0</v>
       </c>
       <c r="O3" s="6">
-        <v>75473224.310000002</v>
+        <v>75957961.340000004</v>
       </c>
       <c r="P3" s="8">
-        <v>0.89333973983451098</v>
+        <v>0.89907733560078829</v>
       </c>
       <c r="Q3" s="6">
-        <v>9011122.4000000004</v>
+        <v>8526385.3699999992</v>
       </c>
       <c r="R3" s="6">
         <v>0</v>
@@ -15751,7 +15749,7 @@
         <v>411572.18</v>
       </c>
       <c r="AN3" s="6">
-        <v>53859.67</v>
+        <v>538596.69999999995</v>
       </c>
       <c r="AO3" s="6">
         <v>0</v>
@@ -15943,13 +15941,13 @@
         <v>0</v>
       </c>
       <c r="O4" s="6">
-        <v>31828130.850000001</v>
+        <v>32682339.390000001</v>
       </c>
       <c r="P4" s="8">
-        <v>0.45828842116630658</v>
+        <v>0.47058804017278622</v>
       </c>
       <c r="Q4" s="6">
-        <v>37621869.149999999</v>
+        <v>36767660.609999999</v>
       </c>
       <c r="R4" s="6">
         <v>0</v>
@@ -16009,13 +16007,13 @@
         <v>2268052.17</v>
       </c>
       <c r="AK4" s="6">
-        <v>52447.55</v>
+        <v>524475.5</v>
       </c>
       <c r="AL4" s="6">
         <v>955557.19</v>
       </c>
       <c r="AM4" s="6">
-        <v>3860.41</v>
+        <v>386041</v>
       </c>
       <c r="AN4" s="6">
         <v>391310.72</v>
@@ -17282,13 +17280,13 @@
         <v>0</v>
       </c>
       <c r="O9" s="6">
-        <v>8075594.0300000003</v>
+        <v>8394719</v>
       </c>
       <c r="P9" s="8">
-        <v>0.96180277536592451</v>
+        <v>0.99981054057729268</v>
       </c>
       <c r="Q9" s="6">
-        <v>320715.73</v>
+        <v>1590.76</v>
       </c>
       <c r="R9" s="6">
         <v>0</v>
@@ -17414,7 +17412,7 @@
         <v>36613.279999999999</v>
       </c>
       <c r="BG9" s="6">
-        <v>35458.33</v>
+        <v>354583.3</v>
       </c>
       <c r="BH9" s="6">
         <v>403701.68</v>
@@ -17551,13 +17549,13 @@
         <v>0</v>
       </c>
       <c r="O10" s="6">
-        <v>3921891.87</v>
+        <v>4374443.7300000004</v>
       </c>
       <c r="P10" s="8">
-        <v>0.89654641075304886</v>
+        <v>0.99999998856997541</v>
       </c>
       <c r="Q10" s="6">
-        <v>452551.91</v>
+        <v>0.05</v>
       </c>
       <c r="R10" s="6">
         <v>0</v>
@@ -17623,7 +17621,7 @@
         <v>107650.53</v>
       </c>
       <c r="AM10" s="6">
-        <v>18318.32</v>
+        <v>183183.2</v>
       </c>
       <c r="AN10" s="6">
         <v>798369.63</v>
@@ -17644,7 +17642,7 @@
         <v>139028.48000000001</v>
       </c>
       <c r="AT10" s="6">
-        <v>31965.22</v>
+        <v>319652.2</v>
       </c>
       <c r="AU10" s="6">
         <v>296228.71999999997</v>
@@ -17820,13 +17818,13 @@
         <v>0</v>
       </c>
       <c r="O11" s="6">
-        <v>1712039.39</v>
+        <v>1740561.74</v>
       </c>
       <c r="P11" s="8">
-        <v>0.9829682280801737</v>
+        <v>0.99934434886567891</v>
       </c>
       <c r="Q11" s="6">
-        <v>29664.3</v>
+        <v>1141.95</v>
       </c>
       <c r="R11" s="6">
         <v>0</v>
@@ -17940,7 +17938,7 @@
         <v>0</v>
       </c>
       <c r="BC11" s="6">
-        <v>3169.15</v>
+        <v>31691.5</v>
       </c>
       <c r="BD11" s="6">
         <v>0</v>
@@ -18089,13 +18087,13 @@
         <v>0</v>
       </c>
       <c r="O12" s="6">
-        <v>6138303.75</v>
+        <v>7104640.0499999998</v>
       </c>
       <c r="P12" s="8">
-        <v>0.69659397427821601</v>
+        <v>0.80625685039546702</v>
       </c>
       <c r="Q12" s="6">
-        <v>2673578.0299999998</v>
+        <v>1707241.73</v>
       </c>
       <c r="R12" s="6">
         <v>0</v>
@@ -18191,7 +18189,7 @@
         <v>686049.52</v>
       </c>
       <c r="AW12" s="6">
-        <v>41612.550000000003</v>
+        <v>416125.5</v>
       </c>
       <c r="AX12" s="6">
         <v>409515.77</v>
@@ -18206,7 +18204,7 @@
         <v>597793.73</v>
       </c>
       <c r="BB12" s="6">
-        <v>11280.52</v>
+        <v>112805.2</v>
       </c>
       <c r="BC12" s="6">
         <v>185864.99</v>
@@ -18224,10 +18222,10 @@
         <v>617746.35</v>
       </c>
       <c r="BH12" s="6">
-        <v>52525.55</v>
+        <v>525255.5</v>
       </c>
       <c r="BI12" s="6">
-        <v>1952.08</v>
+        <v>19520.8</v>
       </c>
       <c r="BJ12" s="6">
         <v>0</v>
@@ -18886,13 +18884,13 @@
         <v>0</v>
       </c>
       <c r="O15" s="6">
-        <v>4942414.46</v>
+        <v>5132338.3099999996</v>
       </c>
       <c r="P15" s="8">
-        <v>0.93746686753608399</v>
+        <v>0.9734912273243751</v>
       </c>
       <c r="Q15" s="6">
-        <v>329680.62</v>
+        <v>139756.76999999999</v>
       </c>
       <c r="R15" s="6">
         <v>0</v>
@@ -19012,7 +19010,7 @@
         <v>0</v>
       </c>
       <c r="BE15" s="6">
-        <v>21102.65</v>
+        <v>211026.5</v>
       </c>
       <c r="BF15" s="6">
         <v>827</v>
@@ -19155,13 +19153,13 @@
         <v>0</v>
       </c>
       <c r="O16" s="6">
-        <v>3542960.18</v>
+        <v>4625557.49</v>
       </c>
       <c r="P16" s="8">
-        <v>0.76272207870043451</v>
+        <v>0.99578167540148965</v>
       </c>
       <c r="Q16" s="6">
-        <v>1102192.07</v>
+        <v>19594.759999999998</v>
       </c>
       <c r="R16" s="6">
         <v>0</v>
@@ -19257,7 +19255,7 @@
         <v>140614.75</v>
       </c>
       <c r="AW16" s="6">
-        <v>31966.85</v>
+        <v>319668.5</v>
       </c>
       <c r="AX16" s="6">
         <v>164215.32999999999</v>
@@ -19281,7 +19279,7 @@
         <v>120984.77</v>
       </c>
       <c r="BE16" s="6">
-        <v>88321.74</v>
+        <v>883217.4</v>
       </c>
       <c r="BF16" s="6">
         <v>492856.12</v>
@@ -19422,13 +19420,13 @@
         <v>0</v>
       </c>
       <c r="O17" s="6">
-        <v>3129510</v>
+        <v>3607318.65</v>
       </c>
       <c r="P17" s="8">
-        <v>0.86753292238803903</v>
+        <v>0.999986480445621</v>
       </c>
       <c r="Q17" s="6">
-        <v>477857.42</v>
+        <v>48.77</v>
       </c>
       <c r="R17" s="6">
         <v>0</v>
@@ -19503,7 +19501,7 @@
         <v>468162.08</v>
       </c>
       <c r="AP17" s="6">
-        <v>4826.3500000000004</v>
+        <v>482635</v>
       </c>
       <c r="AQ17" s="6">
         <v>150829.29</v>
@@ -19691,13 +19689,13 @@
         <v>0</v>
       </c>
       <c r="O18" s="6">
-        <v>10246752.91</v>
+        <v>10939879.359999999</v>
       </c>
       <c r="P18" s="8">
-        <v>0.92759236302966408</v>
+        <v>0.99033797691154146</v>
       </c>
       <c r="Q18" s="6">
-        <v>799859.07</v>
+        <v>106732.62</v>
       </c>
       <c r="R18" s="6">
         <v>0</v>
@@ -19769,7 +19767,7 @@
         <v>484641.18</v>
       </c>
       <c r="AO18" s="6">
-        <v>49045.74</v>
+        <v>490457.4</v>
       </c>
       <c r="AP18" s="6">
         <v>655903.26</v>
@@ -19796,7 +19794,7 @@
         <v>100847.74</v>
       </c>
       <c r="AX18" s="6">
-        <v>27968.31</v>
+        <v>279683.09999999998</v>
       </c>
       <c r="AY18" s="6">
         <v>0</v>
@@ -20227,13 +20225,13 @@
         <v>0</v>
       </c>
       <c r="O20" s="6">
-        <v>5982279.4800000004</v>
+        <v>6171355.1699999999</v>
       </c>
       <c r="P20" s="8">
-        <v>0.19720978979047851</v>
+        <v>0.20344279465159371</v>
       </c>
       <c r="Q20" s="6">
-        <v>24352317.43</v>
+        <v>24163241.739999998</v>
       </c>
       <c r="R20" s="6">
         <v>0</v>
@@ -20317,7 +20315,7 @@
         <v>1076635.31</v>
       </c>
       <c r="AS20" s="6">
-        <v>21008.41</v>
+        <v>210084.1</v>
       </c>
       <c r="AT20" s="6">
         <v>1160220.94</v>
@@ -20490,19 +20488,19 @@
         <v>117</v>
       </c>
       <c r="M21" s="6">
-        <v>2044683.93</v>
+        <v>2214379.38</v>
       </c>
       <c r="N21" s="6">
         <v>0</v>
       </c>
       <c r="O21" s="6">
-        <v>9339511</v>
+        <v>10061305.060000001</v>
       </c>
       <c r="P21" s="8">
-        <v>0.92828804074760951</v>
+        <v>1.0000297833057219</v>
       </c>
       <c r="Q21" s="6">
-        <v>721494.41</v>
+        <v>-299.64999999999998</v>
       </c>
       <c r="R21" s="6">
         <v>0</v>
@@ -20613,7 +20611,7 @@
         <v>163311.32</v>
       </c>
       <c r="BB21" s="6">
-        <v>6790.73</v>
+        <v>67907.3</v>
       </c>
       <c r="BC21" s="6">
         <v>631326.01</v>
@@ -20634,7 +20632,7 @@
         <v>1225723.92</v>
       </c>
       <c r="BI21" s="6">
-        <v>54553.56</v>
+        <v>545535.6</v>
       </c>
       <c r="BJ21" s="6">
         <v>811014.79</v>
@@ -20658,7 +20656,7 @@
         <v>53970.74</v>
       </c>
       <c r="BQ21" s="6">
-        <v>18855.05</v>
+        <v>188550.5</v>
       </c>
       <c r="BR21" s="6">
         <v>1482105.79</v>
@@ -20765,13 +20763,13 @@
         <v>0</v>
       </c>
       <c r="O22" s="6">
-        <v>28986729.09</v>
+        <v>32314427.699999999</v>
       </c>
       <c r="P22" s="8">
-        <v>0.89286723623805864</v>
+        <v>0.9953690760185584</v>
       </c>
       <c r="Q22" s="6">
-        <v>3478040.49</v>
+        <v>150341.88</v>
       </c>
       <c r="R22" s="6">
         <v>0</v>
@@ -20828,7 +20826,7 @@
         <v>531985.32999999996</v>
       </c>
       <c r="AJ22" s="6">
-        <v>94568.14</v>
+        <v>945681.4</v>
       </c>
       <c r="AK22" s="6">
         <v>806675.88</v>
@@ -20843,7 +20841,7 @@
         <v>1228434.6000000001</v>
       </c>
       <c r="AO22" s="6">
-        <v>47189.52</v>
+        <v>471895.2</v>
       </c>
       <c r="AP22" s="6">
         <v>1027729.48</v>
@@ -20867,7 +20865,7 @@
         <v>0</v>
       </c>
       <c r="AW22" s="6">
-        <v>91600.95</v>
+        <v>916009.5</v>
       </c>
       <c r="AX22" s="6">
         <v>641381.87</v>
@@ -20894,10 +20892,10 @@
         <v>1315203.06</v>
       </c>
       <c r="BF22" s="6">
-        <v>90432.66</v>
+        <v>904326.6</v>
       </c>
       <c r="BG22" s="6">
-        <v>45953.02</v>
+        <v>459530.2</v>
       </c>
       <c r="BH22" s="6">
         <v>1726518.92</v>
@@ -21034,13 +21032,13 @@
         <v>0</v>
       </c>
       <c r="O23" s="6">
-        <v>16552659.939999999</v>
+        <v>17677149.640000001</v>
       </c>
       <c r="P23" s="8">
-        <v>0.93543922296812876</v>
+        <v>0.99898742458747924</v>
       </c>
       <c r="Q23" s="6">
-        <v>1142407.29</v>
+        <v>17917.59</v>
       </c>
       <c r="R23" s="6">
         <v>0</v>
@@ -21148,7 +21146,7 @@
         <v>2109380.2200000002</v>
       </c>
       <c r="BA23" s="6">
-        <v>79989.95</v>
+        <v>799899.5</v>
       </c>
       <c r="BB23" s="6">
         <v>1139276.74</v>
@@ -21181,7 +21179,7 @@
         <v>497948.46</v>
       </c>
       <c r="BL23" s="6">
-        <v>44953.35</v>
+        <v>449533.5</v>
       </c>
       <c r="BM23" s="6">
         <v>0</v>
@@ -23172,13 +23170,13 @@
         <v>0</v>
       </c>
       <c r="O31" s="6">
-        <v>3710200.11</v>
+        <v>4324004.79</v>
       </c>
       <c r="P31" s="8">
-        <v>0.83473120996636385</v>
+        <v>0.97282670563476759</v>
       </c>
       <c r="Q31" s="6">
-        <v>734584.11</v>
+        <v>120779.43</v>
       </c>
       <c r="R31" s="6">
         <v>0</v>
@@ -23292,7 +23290,7 @@
         <v>0</v>
       </c>
       <c r="BC31" s="6">
-        <v>68200.52</v>
+        <v>682005.2</v>
       </c>
       <c r="BD31" s="6">
         <v>550395.17000000004</v>
@@ -23708,13 +23706,13 @@
         <v>0</v>
       </c>
       <c r="O33" s="6">
-        <v>2123652.9700000002</v>
+        <v>2226331.4500000002</v>
       </c>
       <c r="P33" s="8">
-        <v>0.77066670438857121</v>
+        <v>0.80792838834121261</v>
       </c>
       <c r="Q33" s="6">
-        <v>631951.96</v>
+        <v>529273.48</v>
       </c>
       <c r="R33" s="6">
         <v>0</v>
@@ -23801,7 +23799,7 @@
         <v>0</v>
       </c>
       <c r="AT33" s="6">
-        <v>8494.2099999999991</v>
+        <v>84942.1</v>
       </c>
       <c r="AU33" s="6">
         <v>264382.34999999998</v>
@@ -23810,7 +23808,7 @@
         <v>28562.41</v>
       </c>
       <c r="AW33" s="6">
-        <v>2914.51</v>
+        <v>29145.1</v>
       </c>
       <c r="AX33" s="6">
         <v>30777.79</v>
@@ -23977,13 +23975,13 @@
         <v>0</v>
       </c>
       <c r="O34" s="6">
-        <v>55344940</v>
+        <v>56408430.850000001</v>
       </c>
       <c r="P34" s="8">
-        <v>0.952799017838179</v>
+        <v>0.97110770219775899</v>
       </c>
       <c r="Q34" s="6">
-        <v>2741748.76</v>
+        <v>1678257.91</v>
       </c>
       <c r="R34" s="6">
         <v>0</v>
@@ -24112,7 +24110,7 @@
         <v>1957520.83</v>
       </c>
       <c r="BH34" s="6">
-        <v>7794.79</v>
+        <v>779479</v>
       </c>
       <c r="BI34" s="6">
         <v>5970935.7800000003</v>
@@ -24124,7 +24122,7 @@
         <v>4118696.93</v>
       </c>
       <c r="BL34" s="6">
-        <v>32422.959999999999</v>
+        <v>324229.59999999998</v>
       </c>
       <c r="BM34" s="6">
         <v>0</v>
@@ -24238,13 +24236,13 @@
         <v>0</v>
       </c>
       <c r="O35" s="6">
-        <v>8661926.9800000004</v>
+        <v>9021796.75</v>
       </c>
       <c r="P35" s="8">
-        <v>0.45596556980537811</v>
+        <v>0.47490918652168768</v>
       </c>
       <c r="Q35" s="6">
-        <v>10334961.279999999</v>
+        <v>9975091.5099999998</v>
       </c>
       <c r="R35" s="6">
         <v>0</v>
@@ -24376,7 +24374,7 @@
         <v>709433.01</v>
       </c>
       <c r="BI35" s="6">
-        <v>360.23</v>
+        <v>360230</v>
       </c>
       <c r="BJ35" s="6">
         <v>5622526.8099999996</v>
@@ -25039,13 +25037,13 @@
         <v>0</v>
       </c>
       <c r="O38" s="6">
-        <v>1883519.36</v>
+        <v>2389346</v>
       </c>
       <c r="P38" s="8">
-        <v>0.78829912453031081</v>
+        <v>1</v>
       </c>
       <c r="Q38" s="6">
-        <v>505826.64</v>
+        <v>0</v>
       </c>
       <c r="R38" s="6">
         <v>0</v>
@@ -25111,7 +25109,7 @@
         <v>739920.75</v>
       </c>
       <c r="AM38" s="6">
-        <v>56202.96</v>
+        <v>562029.6</v>
       </c>
       <c r="AN38" s="6">
         <v>0</v>
@@ -25308,13 +25306,13 @@
         <v>0</v>
       </c>
       <c r="O39" s="6">
-        <v>9228959.0999999996</v>
+        <v>9661616.3699999992</v>
       </c>
       <c r="P39" s="8">
-        <v>0.94640301154504902</v>
+        <v>0.9907707608067029</v>
       </c>
       <c r="Q39" s="6">
-        <v>522657.27</v>
+        <v>90000</v>
       </c>
       <c r="R39" s="6">
         <v>0</v>
@@ -25386,7 +25384,7 @@
         <v>261649.94</v>
       </c>
       <c r="AO39" s="6">
-        <v>6592.96</v>
+        <v>65929.600000000006</v>
       </c>
       <c r="AP39" s="6">
         <v>0</v>
@@ -25422,7 +25420,7 @@
         <v>536257.61</v>
       </c>
       <c r="BA39" s="6">
-        <v>41480.07</v>
+        <v>414800.7</v>
       </c>
       <c r="BB39" s="6">
         <v>0</v>
@@ -25577,13 +25575,13 @@
         <v>0</v>
       </c>
       <c r="O40" s="6">
-        <v>13384606.060000001</v>
+        <v>13792679.65</v>
       </c>
       <c r="P40" s="8">
-        <v>0.97041374582654638</v>
+        <v>0.9999999898496883</v>
       </c>
       <c r="Q40" s="6">
-        <v>408073.73</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="R40" s="6">
         <v>0</v>
@@ -25682,7 +25680,7 @@
         <v>280408.63</v>
       </c>
       <c r="AX40" s="6">
-        <v>30426.959999999999</v>
+        <v>304269.59999999998</v>
       </c>
       <c r="AY40" s="6">
         <v>186166.26</v>
@@ -25700,7 +25698,7 @@
         <v>108879.08</v>
       </c>
       <c r="BD40" s="6">
-        <v>14914.55</v>
+        <v>149145.5</v>
       </c>
       <c r="BE40" s="6">
         <v>0</v>
@@ -25846,13 +25844,13 @@
         <v>0</v>
       </c>
       <c r="O41" s="6">
-        <v>6205092.3799999999</v>
+        <v>6488132.9299999997</v>
       </c>
       <c r="P41" s="8">
-        <v>0.80535046532229959</v>
+        <v>0.84208591174083947</v>
       </c>
       <c r="Q41" s="6">
-        <v>1499742.53</v>
+        <v>1216701.98</v>
       </c>
       <c r="R41" s="6">
         <v>0</v>
@@ -25975,7 +25973,7 @@
         <v>0</v>
       </c>
       <c r="BF41" s="6">
-        <v>31448.95</v>
+        <v>314489.5</v>
       </c>
       <c r="BG41" s="6">
         <v>88206.39</v>
@@ -26641,13 +26639,13 @@
         <v>0</v>
       </c>
       <c r="O44" s="6">
-        <v>5654932.8899999997</v>
+        <v>6453162.3300000001</v>
       </c>
       <c r="P44" s="8">
-        <v>0.87630409077922644</v>
+        <v>0.99999993956451794</v>
       </c>
       <c r="Q44" s="6">
-        <v>798229.83</v>
+        <v>0.39</v>
       </c>
       <c r="R44" s="6">
         <v>0</v>
@@ -26707,7 +26705,7 @@
         <v>991327.11</v>
       </c>
       <c r="AK44" s="6">
-        <v>88692.160000000003</v>
+        <v>886921.6</v>
       </c>
       <c r="AL44" s="6">
         <v>1009464.43</v>
@@ -27984,13 +27982,13 @@
         <v>0</v>
       </c>
       <c r="O49" s="6">
-        <v>5852661.0899999999</v>
+        <v>6450491.3099999996</v>
       </c>
       <c r="P49" s="8">
-        <v>0.80898380280970883</v>
+        <v>0.89161885674039276</v>
       </c>
       <c r="Q49" s="6">
-        <v>1381922.68</v>
+        <v>784092.46</v>
       </c>
       <c r="R49" s="6">
         <v>0</v>
@@ -28122,7 +28120,7 @@
         <v>1940010.25</v>
       </c>
       <c r="BI49" s="6">
-        <v>66425.58</v>
+        <v>664255.80000000005</v>
       </c>
       <c r="BJ49" s="6">
         <v>531746.06000000006</v>
@@ -28253,13 +28251,13 @@
         <v>0</v>
       </c>
       <c r="O50" s="6">
-        <v>9534048.5099999998</v>
+        <v>11566431.390000001</v>
       </c>
       <c r="P50" s="8">
-        <v>0.75906161376384995</v>
+        <v>0.9208715549510299</v>
       </c>
       <c r="Q50" s="6">
-        <v>3026260.61</v>
+        <v>993877.73</v>
       </c>
       <c r="R50" s="6">
         <v>0</v>
@@ -28325,7 +28323,7 @@
         <v>0</v>
       </c>
       <c r="AM50" s="6">
-        <v>53086.16</v>
+        <v>530861.6</v>
       </c>
       <c r="AN50" s="6">
         <v>1760492.78</v>
@@ -28358,7 +28356,7 @@
         <v>836628.45</v>
       </c>
       <c r="AX50" s="6">
-        <v>79864.679999999993</v>
+        <v>798646.8</v>
       </c>
       <c r="AY50" s="6">
         <v>623254.15</v>
@@ -28367,13 +28365,13 @@
         <v>522476.34</v>
       </c>
       <c r="BA50" s="6">
-        <v>4991.45</v>
+        <v>499145</v>
       </c>
       <c r="BB50" s="6">
         <v>308370.59000000003</v>
       </c>
       <c r="BC50" s="6">
-        <v>37963.53</v>
+        <v>379635.3</v>
       </c>
       <c r="BD50" s="6">
         <v>801291.31</v>
@@ -28522,13 +28520,13 @@
         <v>0</v>
       </c>
       <c r="O51" s="6">
-        <v>19435944.559999999</v>
+        <v>20500685.690000001</v>
       </c>
       <c r="P51" s="8">
-        <v>0.86486459152563766</v>
+        <v>0.91224365764898707</v>
       </c>
       <c r="Q51" s="6">
-        <v>3036873.44</v>
+        <v>1972132.31</v>
       </c>
       <c r="R51" s="6">
         <v>0</v>
@@ -28627,7 +28625,7 @@
         <v>325739.93</v>
       </c>
       <c r="AX51" s="6">
-        <v>24635.98</v>
+        <v>246359.8</v>
       </c>
       <c r="AY51" s="6">
         <v>362421.28</v>
@@ -28642,7 +28640,7 @@
         <v>1052655.1299999999</v>
       </c>
       <c r="BC51" s="6">
-        <v>73788.42</v>
+        <v>737884.2</v>
       </c>
       <c r="BD51" s="6">
         <v>885986.93</v>
@@ -28654,7 +28652,7 @@
         <v>522414.47</v>
       </c>
       <c r="BG51" s="6">
-        <v>19880.169999999998</v>
+        <v>198801.7</v>
       </c>
       <c r="BH51" s="6">
         <v>0</v>
@@ -28791,13 +28789,13 @@
         <v>0</v>
       </c>
       <c r="O52" s="6">
-        <v>43141110.719999999</v>
+        <v>43785880.079999998</v>
       </c>
       <c r="P52" s="8">
-        <v>0.95365611266209971</v>
+        <v>0.96790906607843752</v>
       </c>
       <c r="Q52" s="6">
-        <v>2096486.09</v>
+        <v>1451716.73</v>
       </c>
       <c r="R52" s="6">
         <v>0</v>
@@ -28875,7 +28873,7 @@
         <v>1156896.75</v>
       </c>
       <c r="AQ52" s="6">
-        <v>71641.039999999994</v>
+        <v>716410.4</v>
       </c>
       <c r="AR52" s="6">
         <v>788781.45</v>
@@ -29596,13 +29594,13 @@
         <v>0</v>
       </c>
       <c r="O55" s="6">
-        <v>15130.8</v>
+        <v>151308</v>
       </c>
       <c r="P55" s="8">
-        <v>1.316358941562987E-3</v>
+        <v>1.3163589415629879E-2</v>
       </c>
       <c r="Q55" s="6">
-        <v>11479302.460000001</v>
+        <v>11343125.26</v>
       </c>
       <c r="R55" s="6">
         <v>0</v>
@@ -29722,10 +29720,10 @@
         <v>0</v>
       </c>
       <c r="BE55" s="6">
-        <v>8148.54</v>
+        <v>81485.399999999994</v>
       </c>
       <c r="BF55" s="6">
-        <v>6982.26</v>
+        <v>69822.600000000006</v>
       </c>
       <c r="BG55" s="6">
         <v>0</v>
@@ -29865,13 +29863,13 @@
         <v>0</v>
       </c>
       <c r="O56" s="6">
-        <v>12433273.43</v>
+        <v>13332401.6</v>
       </c>
       <c r="P56" s="8">
-        <v>0.61596178074347263</v>
+        <v>0.66050584967494952</v>
       </c>
       <c r="Q56" s="6">
-        <v>7751864.3799999999</v>
+        <v>6852736.21</v>
       </c>
       <c r="R56" s="6">
         <v>0</v>
@@ -29937,10 +29935,10 @@
         <v>459809.72</v>
       </c>
       <c r="AM56" s="6">
-        <v>19028.27</v>
+        <v>190282.7</v>
       </c>
       <c r="AN56" s="6">
-        <v>39634.730000000003</v>
+        <v>396347.3</v>
       </c>
       <c r="AO56" s="6">
         <v>730556.69</v>
@@ -29961,7 +29959,7 @@
         <v>831397.29</v>
       </c>
       <c r="AU56" s="6">
-        <v>41240.129999999997</v>
+        <v>412401.3</v>
       </c>
       <c r="AV56" s="6">
         <v>428339.32</v>
@@ -30134,13 +30132,13 @@
         <v>0</v>
       </c>
       <c r="O57" s="6">
-        <v>11638364.17</v>
+        <v>12534756.699999999</v>
       </c>
       <c r="P57" s="8">
-        <v>0.38186455387351192</v>
+        <v>0.4112759495442489</v>
       </c>
       <c r="Q57" s="6">
-        <v>18839364.260000002</v>
+        <v>17942971.73</v>
       </c>
       <c r="R57" s="6">
         <v>0</v>
@@ -30197,7 +30195,7 @@
         <v>954009.41</v>
       </c>
       <c r="AJ57" s="6">
-        <v>9054.4699999999993</v>
+        <v>905447</v>
       </c>
       <c r="AK57" s="6">
         <v>0</v>
@@ -30403,13 +30401,13 @@
         <v>0</v>
       </c>
       <c r="O58" s="6">
-        <v>5792351.6100000003</v>
+        <v>6523029.6600000001</v>
       </c>
       <c r="P58" s="8">
-        <v>0.89414781249110531</v>
+        <v>1.0069403748270731</v>
       </c>
       <c r="Q58" s="6">
-        <v>685717.82</v>
+        <v>-44960.23</v>
       </c>
       <c r="R58" s="6">
         <v>0</v>
@@ -30496,7 +30494,7 @@
         <v>191164.06</v>
       </c>
       <c r="AT58" s="6">
-        <v>39208.79</v>
+        <v>392087.9</v>
       </c>
       <c r="AU58" s="6">
         <v>176656.04</v>
@@ -30526,7 +30524,7 @@
         <v>61458.43</v>
       </c>
       <c r="BD58" s="6">
-        <v>41977.66</v>
+        <v>419776.6</v>
       </c>
       <c r="BE58" s="6">
         <v>0</v>
@@ -30672,13 +30670,13 @@
         <v>0</v>
       </c>
       <c r="O59" s="6">
-        <v>5144130.55</v>
+        <v>6007931.0199999996</v>
       </c>
       <c r="P59" s="8">
-        <v>0.8495267956923096</v>
+        <v>0.9921790161723304</v>
       </c>
       <c r="Q59" s="6">
-        <v>911158.79</v>
+        <v>47358.32</v>
       </c>
       <c r="R59" s="6">
         <v>0</v>
@@ -30741,7 +30739,7 @@
         <v>1162941.93</v>
       </c>
       <c r="AL59" s="6">
-        <v>95977.83</v>
+        <v>959778.3</v>
       </c>
       <c r="AM59" s="6">
         <v>357381.39</v>
@@ -30941,13 +30939,13 @@
         <v>0</v>
       </c>
       <c r="O60" s="6">
-        <v>4601510.3099999996</v>
+        <v>5551029.21</v>
       </c>
       <c r="P60" s="8">
-        <v>0.80409239807752408</v>
+        <v>0.97001638343982832</v>
       </c>
       <c r="Q60" s="6">
-        <v>1121103.56</v>
+        <v>171584.66</v>
       </c>
       <c r="R60" s="6">
         <v>0</v>
@@ -31037,10 +31035,10 @@
         <v>340146.38</v>
       </c>
       <c r="AU60" s="6">
-        <v>77903.61</v>
+        <v>779036.1</v>
       </c>
       <c r="AV60" s="6">
-        <v>27598.49</v>
+        <v>275984.90000000002</v>
       </c>
       <c r="AW60" s="6">
         <v>49212.09</v>
@@ -31210,13 +31208,13 @@
         <v>0</v>
       </c>
       <c r="O61" s="6">
-        <v>4936315.0199999996</v>
+        <v>5580983.9400000004</v>
       </c>
       <c r="P61" s="8">
-        <v>0.88436987642167575</v>
+        <v>0.99986610605924364</v>
       </c>
       <c r="Q61" s="6">
-        <v>645416.28</v>
+        <v>747.36</v>
       </c>
       <c r="R61" s="6">
         <v>0</v>
@@ -31309,7 +31307,7 @@
         <v>46981.97</v>
       </c>
       <c r="AV61" s="6">
-        <v>13789.46</v>
+        <v>137894.6</v>
       </c>
       <c r="AW61" s="6">
         <v>92670.48</v>
@@ -31327,7 +31325,7 @@
         <v>0</v>
       </c>
       <c r="BB61" s="6">
-        <v>5258.22</v>
+        <v>525822</v>
       </c>
       <c r="BC61" s="6">
         <v>0</v>
@@ -31479,13 +31477,13 @@
         <v>0</v>
       </c>
       <c r="O62" s="6">
-        <v>11186461.67</v>
+        <v>12032786.93</v>
       </c>
       <c r="P62" s="8">
-        <v>0.84689261033914798</v>
+        <v>0.91096529299621554</v>
       </c>
       <c r="Q62" s="6">
-        <v>2022369.69</v>
+        <v>1176044.43</v>
       </c>
       <c r="R62" s="6">
         <v>0</v>
@@ -31569,7 +31567,7 @@
         <v>1476783.27</v>
       </c>
       <c r="AS62" s="6">
-        <v>94036.14</v>
+        <v>940361.4</v>
       </c>
       <c r="AT62" s="6">
         <v>603293.64</v>
@@ -32017,13 +32015,13 @@
         <v>0</v>
       </c>
       <c r="O64" s="6">
-        <v>8494636.8499999996</v>
+        <v>8552770.9100000001</v>
       </c>
       <c r="P64" s="8">
-        <v>0.65593763466600818</v>
+        <v>0.6604266220686813</v>
       </c>
       <c r="Q64" s="6">
-        <v>4455735.87</v>
+        <v>4397601.8099999996</v>
       </c>
       <c r="R64" s="6">
         <v>0</v>
@@ -32113,7 +32111,7 @@
         <v>0</v>
       </c>
       <c r="AU64" s="6">
-        <v>6459.34</v>
+        <v>64593.4</v>
       </c>
       <c r="AV64" s="6">
         <v>59504.88</v>
@@ -32549,19 +32547,19 @@
         <v>142</v>
       </c>
       <c r="M66" s="6">
-        <v>12776757.41</v>
+        <v>14479558.67</v>
       </c>
       <c r="N66" s="6">
         <v>0</v>
       </c>
       <c r="O66" s="6">
-        <v>80256809.739999995</v>
+        <v>81959611</v>
       </c>
       <c r="P66" s="8">
-        <v>0.97932703787168673</v>
+        <v>1.0001053284546579</v>
       </c>
       <c r="Q66" s="6">
-        <v>1694169.49</v>
+        <v>-8631.77</v>
       </c>
       <c r="R66" s="6">
         <v>0</v>
@@ -32711,7 +32709,7 @@
         <v>344977.36</v>
       </c>
       <c r="BO66" s="6">
-        <v>90293.61</v>
+        <v>902936.1</v>
       </c>
       <c r="BP66" s="6">
         <v>2195846.5499999998</v>
@@ -32732,7 +32730,7 @@
         <v>1106666.3700000001</v>
       </c>
       <c r="BV66" s="6">
-        <v>98906.53</v>
+        <v>989065.3</v>
       </c>
       <c r="BW66" s="6">
         <v>1004285.95</v>
@@ -32822,13 +32820,13 @@
         <v>0</v>
       </c>
       <c r="O67" s="6">
-        <v>1674266.74</v>
+        <v>2042159.29</v>
       </c>
       <c r="P67" s="8">
-        <v>0.1865689491149041</v>
+        <v>0.22756440390169769</v>
       </c>
       <c r="Q67" s="6">
-        <v>7299717.1299999999</v>
+        <v>6931824.5800000001</v>
       </c>
       <c r="R67" s="6">
         <v>0</v>
@@ -32891,7 +32889,7 @@
         <v>679501.38</v>
       </c>
       <c r="AL67" s="6">
-        <v>40876.949999999997</v>
+        <v>408769.5</v>
       </c>
       <c r="AM67" s="6">
         <v>382552.94</v>
@@ -33089,13 +33087,13 @@
         <v>0</v>
       </c>
       <c r="O68" s="6">
-        <v>3334970.55</v>
+        <v>4852080.3</v>
       </c>
       <c r="P68" s="8">
-        <v>0.27957247285910358</v>
+        <v>0.40675264373232362</v>
       </c>
       <c r="Q68" s="6">
-        <v>8593852.4700000007</v>
+        <v>7076742.7199999997</v>
       </c>
       <c r="R68" s="6">
         <v>0</v>
@@ -33173,7 +33171,7 @@
         <v>719239.45</v>
       </c>
       <c r="AQ68" s="6">
-        <v>721.48</v>
+        <v>721480</v>
       </c>
       <c r="AR68" s="6">
         <v>611174.84</v>
@@ -33185,7 +33183,7 @@
         <v>711229.41</v>
       </c>
       <c r="AU68" s="6">
-        <v>88483.47</v>
+        <v>884834.7</v>
       </c>
       <c r="AV68" s="6">
         <v>0</v>
@@ -33358,13 +33356,13 @@
         <v>0</v>
       </c>
       <c r="O69" s="6">
-        <v>10511349.710000001</v>
+        <v>11551184.42</v>
       </c>
       <c r="P69" s="8">
-        <v>0.9099802504755089</v>
+        <v>0.99999999826857588</v>
       </c>
       <c r="Q69" s="6">
-        <v>1039834.73</v>
+        <v>0.02</v>
       </c>
       <c r="R69" s="6">
         <v>0</v>
@@ -33424,7 +33422,7 @@
         <v>120478.62</v>
       </c>
       <c r="AK69" s="6">
-        <v>35765.370000000003</v>
+        <v>357653.7</v>
       </c>
       <c r="AL69" s="6">
         <v>730489.17</v>
@@ -33457,7 +33455,7 @@
         <v>743481.86</v>
       </c>
       <c r="AV69" s="6">
-        <v>20575.07</v>
+        <v>205750.7</v>
       </c>
       <c r="AW69" s="6">
         <v>207806.97</v>
@@ -33478,7 +33476,7 @@
         <v>1898281</v>
       </c>
       <c r="BC69" s="6">
-        <v>59196.75</v>
+        <v>591967.5</v>
       </c>
       <c r="BD69" s="6">
         <v>307578.92</v>
@@ -33894,13 +33892,13 @@
         <v>0</v>
       </c>
       <c r="O71" s="6">
-        <v>1284066.97</v>
+        <v>1496414.32</v>
       </c>
       <c r="P71" s="8">
-        <v>0.85673378618960183</v>
+        <v>0.99841264983394018</v>
       </c>
       <c r="Q71" s="6">
-        <v>214726.46</v>
+        <v>2379.11</v>
       </c>
       <c r="R71" s="6">
         <v>0</v>
@@ -33969,7 +33967,7 @@
         <v>160691.98000000001</v>
       </c>
       <c r="AN71" s="6">
-        <v>23594.15</v>
+        <v>235941.5</v>
       </c>
       <c r="AO71" s="6">
         <v>293959.24</v>
@@ -34699,13 +34697,13 @@
         <v>0</v>
       </c>
       <c r="O74" s="6">
-        <v>17793137.829999998</v>
+        <v>18264452.890000001</v>
       </c>
       <c r="P74" s="8">
-        <v>0.97419495328775751</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="Q74" s="6">
-        <v>471315.06</v>
+        <v>0</v>
       </c>
       <c r="R74" s="6">
         <v>0</v>
@@ -34843,7 +34841,7 @@
         <v>371421.96</v>
       </c>
       <c r="BK74" s="6">
-        <v>52368.34</v>
+        <v>523683.4</v>
       </c>
       <c r="BL74" s="6">
         <v>595765.34</v>
@@ -35237,13 +35235,13 @@
         <v>0</v>
       </c>
       <c r="O76" s="6">
-        <v>34668428.539999999</v>
+        <v>35196032.93</v>
       </c>
       <c r="P76" s="8">
-        <v>0.9400279846570283</v>
+        <v>0.95433387945279813</v>
       </c>
       <c r="Q76" s="6">
-        <v>2211780.46</v>
+        <v>1684176.07</v>
       </c>
       <c r="R76" s="6">
         <v>0</v>
@@ -35315,7 +35313,7 @@
         <v>2115661.2400000002</v>
       </c>
       <c r="AO76" s="6">
-        <v>58622.71</v>
+        <v>586227.1</v>
       </c>
       <c r="AP76" s="6">
         <v>646953.63</v>
@@ -35506,13 +35504,13 @@
         <v>0</v>
       </c>
       <c r="O77" s="6">
-        <v>18836010.379999999</v>
+        <v>19910338.670000002</v>
       </c>
       <c r="P77" s="8">
-        <v>0.93113208293664051</v>
+        <v>0.98424001387554128</v>
       </c>
       <c r="Q77" s="6">
-        <v>1393139.41</v>
+        <v>318811.12</v>
       </c>
       <c r="R77" s="6">
         <v>0</v>
@@ -35602,7 +35600,7 @@
         <v>483077.81</v>
       </c>
       <c r="AU77" s="6">
-        <v>50401.74</v>
+        <v>504017.4</v>
       </c>
       <c r="AV77" s="6">
         <v>498014.43</v>
@@ -35647,7 +35645,7 @@
         <v>848344.54</v>
       </c>
       <c r="BJ77" s="6">
-        <v>68968.070000000007</v>
+        <v>689680.7</v>
       </c>
       <c r="BK77" s="6">
         <v>398856.19</v>
@@ -37897,13 +37895,13 @@
         <v>0</v>
       </c>
       <c r="O86" s="6">
-        <v>12334318.960000001</v>
+        <v>12576165.07</v>
       </c>
       <c r="P86" s="8">
-        <v>0.54193040342855758</v>
+        <v>0.5525563455973117</v>
       </c>
       <c r="Q86" s="6">
-        <v>10425649.630000001</v>
+        <v>10183803.52</v>
       </c>
       <c r="R86" s="6">
         <v>0</v>
@@ -37939,7 +37937,7 @@
         <v>4651203.96</v>
       </c>
       <c r="AC86" s="6">
-        <v>2442.89</v>
+        <v>244289</v>
       </c>
       <c r="AD86" s="6">
         <v>223327.48</v>
@@ -38433,13 +38431,13 @@
         <v>0</v>
       </c>
       <c r="O88" s="6">
-        <v>4991166.83</v>
+        <v>5260332.26</v>
       </c>
       <c r="P88" s="8">
-        <v>0.93949862345464275</v>
+        <v>0.99016424125098834</v>
       </c>
       <c r="Q88" s="6">
-        <v>321418.74</v>
+        <v>52253.31</v>
       </c>
       <c r="R88" s="6">
         <v>0</v>
@@ -38520,7 +38518,7 @@
         <v>0</v>
       </c>
       <c r="AR88" s="6">
-        <v>29907.27</v>
+        <v>299072.7</v>
       </c>
       <c r="AS88" s="6">
         <v>361569.46</v>
@@ -38702,13 +38700,13 @@
         <v>0</v>
       </c>
       <c r="O89" s="6">
-        <v>5316529.71</v>
+        <v>5319860.7</v>
       </c>
       <c r="P89" s="8">
-        <v>0.99162230345055302</v>
+        <v>0.99224358916825672</v>
       </c>
       <c r="Q89" s="6">
-        <v>44916.57</v>
+        <v>41585.58</v>
       </c>
       <c r="R89" s="6">
         <v>0</v>
@@ -38798,13 +38796,13 @@
         <v>3981.23</v>
       </c>
       <c r="AU89" s="6">
-        <v>172.63</v>
+        <v>1726.3</v>
       </c>
       <c r="AV89" s="6">
         <v>2318.7399999999998</v>
       </c>
       <c r="AW89" s="6">
-        <v>197.48</v>
+        <v>1974.8</v>
       </c>
       <c r="AX89" s="6">
         <v>1382.36</v>
@@ -40290,19 +40288,19 @@
         <v>385</v>
       </c>
       <c r="M95" s="6">
-        <v>3832747.11</v>
+        <v>4600873.3499999996</v>
       </c>
       <c r="N95" s="6">
         <v>0</v>
       </c>
       <c r="O95" s="6">
-        <v>5223570.42</v>
+        <v>5991696.6600000001</v>
       </c>
       <c r="P95" s="8">
-        <v>0.77206967705496121</v>
+        <v>0.88560255406636013</v>
       </c>
       <c r="Q95" s="6">
-        <v>1542101.87</v>
+        <v>773975.63</v>
       </c>
       <c r="R95" s="6">
         <v>0</v>
@@ -40461,7 +40459,7 @@
         <v>1778629.34</v>
       </c>
       <c r="BR95" s="6">
-        <v>85347.36</v>
+        <v>853473.6</v>
       </c>
       <c r="BS95" s="6">
         <v>791806.64</v>
@@ -41366,13 +41364,13 @@
         <v>0</v>
       </c>
       <c r="O99" s="6">
-        <v>1696089.15</v>
+        <v>1923627.24</v>
       </c>
       <c r="P99" s="8">
-        <v>0.88171404706097878</v>
+        <v>1.000000005198513</v>
       </c>
       <c r="Q99" s="6">
-        <v>227538.08</v>
+        <v>-0.01</v>
       </c>
       <c r="R99" s="6">
         <v>0</v>
@@ -41459,7 +41457,7 @@
         <v>132786.18</v>
       </c>
       <c r="AT99" s="6">
-        <v>17018.28</v>
+        <v>170182.8</v>
       </c>
       <c r="AU99" s="6">
         <v>136974.88</v>
@@ -41504,7 +41502,7 @@
         <v>79200.210000000006</v>
       </c>
       <c r="BI99" s="6">
-        <v>8263.73</v>
+        <v>82637.3</v>
       </c>
       <c r="BJ99" s="6">
         <v>113915.66</v>
@@ -42173,13 +42171,13 @@
         <v>0</v>
       </c>
       <c r="O102" s="6">
-        <v>29632883.07</v>
+        <v>30456294.329999998</v>
       </c>
       <c r="P102" s="8">
-        <v>0.96839490289905084</v>
+        <v>0.99530376847551405</v>
       </c>
       <c r="Q102" s="6">
-        <v>967115.94</v>
+        <v>143704.68</v>
       </c>
       <c r="R102" s="6">
         <v>0</v>
@@ -42269,7 +42267,7 @@
         <v>1414040.86</v>
       </c>
       <c r="AU102" s="6">
-        <v>91490.14</v>
+        <v>914901.4</v>
       </c>
       <c r="AV102" s="6">
         <v>118615.88</v>
@@ -42709,13 +42707,13 @@
         <v>0</v>
       </c>
       <c r="O104" s="6">
-        <v>25241861.489999998</v>
+        <v>26930984.010000002</v>
       </c>
       <c r="P104" s="8">
-        <v>0.93673296134625372</v>
+        <v>0.99941679870361666</v>
       </c>
       <c r="Q104" s="6">
-        <v>1704837.87</v>
+        <v>15715.35</v>
       </c>
       <c r="R104" s="6">
         <v>0</v>
@@ -42811,7 +42809,7 @@
         <v>2020437.14</v>
       </c>
       <c r="AW104" s="6">
-        <v>89078.82</v>
+        <v>890788.2</v>
       </c>
       <c r="AX104" s="6">
         <v>274255.71999999997</v>
@@ -42844,7 +42842,7 @@
         <v>1445406.25</v>
       </c>
       <c r="BH104" s="6">
-        <v>98601.46</v>
+        <v>986014.6</v>
       </c>
       <c r="BI104" s="6">
         <v>1196482.33</v>
@@ -43247,13 +43245,13 @@
         <v>0</v>
       </c>
       <c r="O106" s="6">
-        <v>2921910.03</v>
+        <v>3538001.16</v>
       </c>
       <c r="P106" s="8">
-        <v>0.81864670065036704</v>
+        <v>0.99126015065260953</v>
       </c>
       <c r="Q106" s="6">
-        <v>647285.36</v>
+        <v>31194.23</v>
       </c>
       <c r="R106" s="6">
         <v>0</v>
@@ -43304,7 +43302,7 @@
         <v>347400.67</v>
       </c>
       <c r="AH106" s="6">
-        <v>64528.22</v>
+        <v>645282.19999999995</v>
       </c>
       <c r="AI106" s="6">
         <v>510653.43</v>
@@ -43319,7 +43317,7 @@
         <v>903704.06</v>
       </c>
       <c r="AM106" s="6">
-        <v>3926.35</v>
+        <v>39263.5</v>
       </c>
       <c r="AN106" s="6">
         <v>0</v>
@@ -43781,13 +43779,13 @@
         <v>0</v>
       </c>
       <c r="O108" s="6">
-        <v>633410.98</v>
+        <v>724764.22</v>
       </c>
       <c r="P108" s="8">
         <v>0</v>
       </c>
       <c r="Q108" s="6">
-        <v>-633410.98</v>
+        <v>-724764.22</v>
       </c>
       <c r="R108" s="6">
         <v>0</v>
@@ -43877,7 +43875,7 @@
         <v>114920.76</v>
       </c>
       <c r="AU108" s="6">
-        <v>10150.36</v>
+        <v>101503.6</v>
       </c>
       <c r="AV108" s="6">
         <v>0</v>
@@ -46736,13 +46734,13 @@
         <v>0</v>
       </c>
       <c r="O119" s="6">
-        <v>12688117.140000001</v>
+        <v>13048536.539999999</v>
       </c>
       <c r="P119" s="8">
-        <v>0.75165502030776821</v>
+        <v>0.7730065769207074</v>
       </c>
       <c r="Q119" s="6">
-        <v>4192122.86</v>
+        <v>3831703.46</v>
       </c>
       <c r="R119" s="6">
         <v>0</v>
@@ -46802,10 +46800,10 @@
         <v>679932.12</v>
       </c>
       <c r="AK119" s="6">
-        <v>19408.98</v>
+        <v>194089.8</v>
       </c>
       <c r="AL119" s="6">
-        <v>20637.62</v>
+        <v>206376.2</v>
       </c>
       <c r="AM119" s="6">
         <v>0</v>
@@ -47543,13 +47541,13 @@
         <v>0</v>
       </c>
       <c r="O122" s="6">
-        <v>7956304.1900000004</v>
+        <v>8398407.2300000004</v>
       </c>
       <c r="P122" s="8">
-        <v>0.3292433358081146</v>
+        <v>0.34753819686225279</v>
       </c>
       <c r="Q122" s="6">
-        <v>16209117.93</v>
+        <v>15767014.890000001</v>
       </c>
       <c r="R122" s="6">
         <v>0</v>
@@ -47591,7 +47589,7 @@
         <v>85270.45</v>
       </c>
       <c r="AE122" s="6">
-        <v>18349.72</v>
+        <v>183497.2</v>
       </c>
       <c r="AF122" s="6">
         <v>269577.71999999997</v>
@@ -47600,7 +47598,7 @@
         <v>270437.77</v>
       </c>
       <c r="AH122" s="6">
-        <v>27379.919999999998</v>
+        <v>273799.2</v>
       </c>
       <c r="AI122" s="6">
         <v>371021.51</v>
@@ -47648,7 +47646,7 @@
         <v>133423.93</v>
       </c>
       <c r="AX122" s="6">
-        <v>3392.92</v>
+        <v>33929.199999999997</v>
       </c>
       <c r="AY122" s="6">
         <v>1505821.47</v>
@@ -47812,13 +47810,13 @@
         <v>0</v>
       </c>
       <c r="O123" s="6">
-        <v>242119.4</v>
+        <v>255684.47</v>
       </c>
       <c r="P123" s="8">
-        <v>6.6960462461981507E-2</v>
+        <v>7.0712013806190813E-2</v>
       </c>
       <c r="Q123" s="6">
-        <v>3373736.75</v>
+        <v>3360171.68</v>
       </c>
       <c r="R123" s="6">
         <v>0</v>
@@ -47920,7 +47918,7 @@
         <v>6051.68</v>
       </c>
       <c r="AY123" s="6">
-        <v>1507.23</v>
+        <v>15072.3</v>
       </c>
       <c r="AZ123" s="6">
         <v>4019.97</v>
@@ -48081,13 +48079,13 @@
         <v>0</v>
       </c>
       <c r="O124" s="6">
-        <v>12874385.859999999</v>
+        <v>14985593.439999999</v>
       </c>
       <c r="P124" s="8">
-        <v>0.85857347159456221</v>
+        <v>0.99936673668141063</v>
       </c>
       <c r="Q124" s="6">
-        <v>2120703.42</v>
+        <v>9495.84</v>
       </c>
       <c r="R124" s="6">
         <v>0</v>
@@ -48141,7 +48139,7 @@
         <v>0</v>
       </c>
       <c r="AI124" s="6">
-        <v>90637.71</v>
+        <v>906377.1</v>
       </c>
       <c r="AJ124" s="6">
         <v>0</v>
@@ -48156,7 +48154,7 @@
         <v>1077897.6200000001</v>
       </c>
       <c r="AN124" s="6">
-        <v>96623.360000000001</v>
+        <v>966233.59999999998</v>
       </c>
       <c r="AO124" s="6">
         <v>0</v>
@@ -48204,7 +48202,7 @@
         <v>60941.37</v>
       </c>
       <c r="BD124" s="6">
-        <v>47317.55</v>
+        <v>473175.5</v>
       </c>
       <c r="BE124" s="6">
         <v>1022166.32</v>
@@ -48619,13 +48617,13 @@
         <v>0</v>
       </c>
       <c r="O126" s="6">
-        <v>20224500.370000001</v>
+        <v>21925638.52</v>
       </c>
       <c r="P126" s="8">
-        <v>0.82243979237899134</v>
+        <v>0.8916174571567731</v>
       </c>
       <c r="Q126" s="6">
-        <v>4366357.9000000004</v>
+        <v>2665219.75</v>
       </c>
       <c r="R126" s="6">
         <v>0</v>
@@ -48670,10 +48668,10 @@
         <v>0</v>
       </c>
       <c r="AF126" s="6">
-        <v>8218.85</v>
+        <v>821885</v>
       </c>
       <c r="AG126" s="6">
-        <v>66603.47</v>
+        <v>666034.69999999995</v>
       </c>
       <c r="AH126" s="6">
         <v>1095907.96</v>
@@ -48733,7 +48731,7 @@
         <v>1471882.58</v>
       </c>
       <c r="BA126" s="6">
-        <v>32004.53</v>
+        <v>320045.3</v>
       </c>
       <c r="BB126" s="6">
         <v>106063.07</v>
@@ -49120,7 +49118,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
chore: Update `BASE.xlsx` spreadsheet content.
</commit_message>
<xml_diff>
--- a/MEDIÇÕES_CONSOLIDADO.xlsx
+++ b/MEDIÇÕES_CONSOLIDADO.xlsx
@@ -2,24 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
-  <workbookPr/>
+  <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APRENDIZADO APP\MEDICOES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3622BA-9575-4876-9CD9-68494AFD448D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81761B4C-8D9B-4612-B40A-5BD3399AE980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Medições" sheetId="1" r:id="rId1"/>
     <sheet name="PROBLEMAS" sheetId="2" r:id="rId2"/>
     <sheet name="GESTOR_FALTANTES" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Medições!$A$1:$CK$49</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1571,7 +1568,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{FA7612CA-BB5F-4472-8802-45E6C239BFB6}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{5BFDF7BA-2735-4232-A424-D5F1C9F7D8D7}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1869,9 +1866,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:CK49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10262,16 +10262,16 @@
         <v>6197590.2599999998</v>
       </c>
       <c r="N32" s="6">
-        <v>0</v>
+        <v>3545422.68</v>
       </c>
       <c r="O32" s="6">
-        <v>15889085.539999999</v>
+        <v>19434508.219999999</v>
       </c>
       <c r="P32" s="8">
-        <v>0.7902647465307262</v>
+        <v>0.96660104659664492</v>
       </c>
       <c r="Q32" s="6">
-        <v>4216942.99</v>
+        <v>671520.31</v>
       </c>
       <c r="R32" s="6">
         <v>0</v>
@@ -10454,10 +10454,10 @@
         <v>1527833.15</v>
       </c>
       <c r="BZ32" s="6">
-        <v>0</v>
+        <v>537831.15</v>
       </c>
       <c r="CA32" s="6">
-        <v>0</v>
+        <v>3007591.53</v>
       </c>
       <c r="CB32" s="6">
         <v>0</v>
@@ -15064,13 +15064,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:CK49" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Planilha2"/>
   <dimension ref="A1:CK127"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -49118,6 +49118,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Planilha3"/>
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>